<commit_message>
Growth Constraints on ELC, and some refinements to ELC
</commit_message>
<xml_diff>
--- a/suppxls/Scen_UC_ELC.xlsx
+++ b/suppxls/Scen_UC_ELC.xlsx
@@ -8,20 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\suppxls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A99DB5E1-5C23-4C0F-91CD-2F8F9D086743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51FE3693-826C-454E-B3BE-DB87769AC88C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2175" yWindow="-13680" windowWidth="21600" windowHeight="11385" xr2:uid="{22D7DAD2-FC1B-44BE-801D-D5E60FB61EEE}"/>
+    <workbookView xWindow="1890" yWindow="1170" windowWidth="26610" windowHeight="13740" firstSheet="1" activeTab="4" xr2:uid="{22D7DAD2-FC1B-44BE-801D-D5E60FB61EEE}"/>
   </bookViews>
   <sheets>
     <sheet name="BuildRateConstraints" sheetId="1" r:id="rId1"/>
+    <sheet name="TransDum" sheetId="4" r:id="rId2"/>
+    <sheet name="BatteryConstraint" sheetId="5" r:id="rId3"/>
+    <sheet name="FIRMConstraint" sheetId="3" r:id="rId4"/>
+    <sheet name="WindPVConstraint" sheetId="8" r:id="rId5"/>
+    <sheet name="WindThermalConstraint" sheetId="6" r:id="rId6"/>
+    <sheet name="GrowthConstraints" sheetId="7" r:id="rId7"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
-    <externalReference r:id="rId3"/>
-    <externalReference r:id="rId4"/>
-    <externalReference r:id="rId5"/>
-    <externalReference r:id="rId6"/>
-    <externalReference r:id="rId7"/>
     <externalReference r:id="rId8"/>
     <externalReference r:id="rId9"/>
     <externalReference r:id="rId10"/>
@@ -30,6 +30,12 @@
     <externalReference r:id="rId13"/>
     <externalReference r:id="rId14"/>
     <externalReference r:id="rId15"/>
+    <externalReference r:id="rId16"/>
+    <externalReference r:id="rId17"/>
+    <externalReference r:id="rId18"/>
+    <externalReference r:id="rId19"/>
+    <externalReference r:id="rId20"/>
+    <externalReference r:id="rId21"/>
   </externalReferences>
   <definedNames>
     <definedName name="\I">#REF!</definedName>
@@ -1825,6 +1831,12 @@
     <definedName name="LOADFACTOR">#REF!</definedName>
     <definedName name="LOADFACTOR2">#REF!</definedName>
     <definedName name="LOADFACTOR3">#REF!</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="2" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="3" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="6" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="1" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="4" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="5" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="Model_RUN_code">[7]Index!$A$2</definedName>
     <definedName name="monthlydel">#REF!</definedName>
@@ -2005,7 +2017,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="48">
   <si>
     <t>UP</t>
   </si>
@@ -2066,12 +2078,96 @@
   <si>
     <t>UC - Each Region/Period</t>
   </si>
+  <si>
+    <t>UCCAP_DUMETR</t>
+  </si>
+  <si>
+    <t>ETRANS*</t>
+  </si>
+  <si>
+    <t>LO</t>
+  </si>
+  <si>
+    <t>ET*,ER*,EPT*,-ETRANS*,-ERSOLPR*</t>
+  </si>
+  <si>
+    <t>UC_CAP</t>
+  </si>
+  <si>
+    <t>UCCAP_BATTR</t>
+  </si>
+  <si>
+    <t>ET*,-ETRAN*</t>
+  </si>
+  <si>
+    <t>ESTSU*,ERSOLT*</t>
+  </si>
+  <si>
+    <t>Average CF</t>
+  </si>
+  <si>
+    <t>Worst 10% of the year</t>
+  </si>
+  <si>
+    <t>Diff</t>
+  </si>
+  <si>
+    <t>ERW*</t>
+  </si>
+  <si>
+    <t>UC_ACT</t>
+  </si>
+  <si>
+    <t>UCACT_WIND</t>
+  </si>
+  <si>
+    <t>UC_Growth_Wind</t>
+  </si>
+  <si>
+    <t>UC_ATTR</t>
+  </si>
+  <si>
+    <t>NCAP,GROWTH</t>
+  </si>
+  <si>
+    <t>Max growth rate</t>
+  </si>
+  <si>
+    <t>Starting Value (GW)</t>
+  </si>
+  <si>
+    <t>UC_NCAP~RHS</t>
+  </si>
+  <si>
+    <t>UC_RHSRT~0</t>
+  </si>
+  <si>
+    <t>ERSOLP*</t>
+  </si>
+  <si>
+    <t>UC_Growth_Solar</t>
+  </si>
+  <si>
+    <t>UC_Growth_Batteries</t>
+  </si>
+  <si>
+    <t>ESTSUTL</t>
+  </si>
+  <si>
+    <t>UC_RHSRT</t>
+  </si>
+  <si>
+    <t>UCCAP_WIND</t>
+  </si>
+  <si>
+    <t>Year Start</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2102,8 +2198,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2128,8 +2230,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -2137,11 +2245,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2152,6 +2269,12 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2167,6 +2290,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>208687</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>151912</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A56E4996-2CDB-BE2B-BFA0-EE146A133BA3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12163425" y="381000"/>
+          <a:ext cx="6904762" cy="3904762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -19801,8 +19973,8 @@
   </sheetPr>
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6:M9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -19825,8 +19997,173 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
-      <c r="J4" t="s">
+    <row r="5" spans="1:13">
+      <c r="B5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="15">
+      <c r="B6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>3</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15">
+      <c r="B7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>2020</v>
+      </c>
+      <c r="J7" t="s">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>2</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="15">
+      <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8">
+        <v>2030</v>
+      </c>
+      <c r="J8" t="s">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>5</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15">
+      <c r="B9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <v>2050</v>
+      </c>
+      <c r="J9" t="s">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>100</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48D68093-CC56-41C9-9331-EF6093F22379}">
+  <sheetPr>
+    <tabColor theme="8"/>
+  </sheetPr>
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.28515625" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15">
+      <c r="B2" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15">
+      <c r="B3" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="15">
+      <c r="J4" s="8" t="s">
         <v>16</v>
       </c>
     </row>
@@ -19859,7 +20196,7 @@
         <v>7</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="L5" s="3" t="s">
         <v>5</v>
@@ -19868,93 +20205,1074 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15">
-      <c r="B6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>2</v>
+    <row r="6" spans="1:13">
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
+      <c r="J6" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="K6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L6">
         <v>3</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7">
+        <v>3</v>
+      </c>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8">
+        <v>2017</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8">
         <v>1</v>
       </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9">
+        <v>2017</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9">
+        <v>-1</v>
+      </c>
+      <c r="M9" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B4F7123-87B7-410A-B377-BFFE5072DE8B}">
+  <sheetPr>
+    <tabColor theme="8"/>
+  </sheetPr>
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.28515625" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15">
+      <c r="B2" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15">
+      <c r="B3" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="15">
+      <c r="J4" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="B5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="B6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6">
+        <v>3</v>
+      </c>
+      <c r="L6">
+        <v>3</v>
+      </c>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="B7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7">
+        <v>3</v>
+      </c>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="B8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="2" t="str">
+        <f>D6</f>
+        <v>ESTSU*,ERSOLT*</v>
+      </c>
+      <c r="I8">
+        <v>2017</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8">
+        <v>-1</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="B9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="2" t="str">
+        <f>D7</f>
+        <v>ET*,-ETRAN*</v>
+      </c>
+      <c r="I9">
+        <v>2017</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="M9" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8F11F6D-537E-46F8-8C46-53B9A092383F}">
+  <sheetPr>
+    <tabColor theme="8"/>
+  </sheetPr>
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:N9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15">
+      <c r="B2" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15">
+      <c r="B3" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="B5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="15">
+      <c r="B6" s="2"/>
+      <c r="D6" s="1"/>
+      <c r="M6" s="2"/>
     </row>
     <row r="7" spans="1:13" ht="15">
-      <c r="B7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I7">
-        <v>2020</v>
-      </c>
-      <c r="J7" t="s">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>1</v>
-      </c>
-      <c r="L7">
-        <v>2</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="B7" s="2"/>
+      <c r="D7" s="1"/>
+      <c r="M7" s="2"/>
     </row>
     <row r="8" spans="1:13" ht="15">
+      <c r="B8" s="2"/>
+      <c r="D8" s="1"/>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="1:13" ht="15">
+      <c r="B9" s="2"/>
+      <c r="D9" s="1"/>
+      <c r="M9" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC6B3732-8682-4CBF-9448-8AEF3ED05AEF}">
+  <sheetPr>
+    <tabColor theme="8"/>
+  </sheetPr>
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.28515625" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="9"/>
+    </row>
+    <row r="2" spans="1:13" ht="15">
+      <c r="B2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="9"/>
+    </row>
+    <row r="3" spans="1:13" ht="15">
+      <c r="B3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="9"/>
+    </row>
+    <row r="4" spans="1:13" ht="15">
+      <c r="J4" s="8"/>
+      <c r="K4" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="B5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="B6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6">
+        <v>5</v>
+      </c>
+      <c r="L6">
+        <v>5</v>
+      </c>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="B7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7">
+        <v>5</v>
+      </c>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:13">
       <c r="B8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>2</v>
+        <v>46</v>
+      </c>
+      <c r="D8" s="2" t="str">
+        <f>D6</f>
+        <v>ERSOLPC*</v>
       </c>
       <c r="I8">
         <v>2030</v>
       </c>
-      <c r="J8" t="s">
-        <v>0</v>
+      <c r="J8" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="K8">
         <v>1</v>
       </c>
       <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="B9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="2" t="str">
+        <f>D7</f>
+        <v>ERW*</v>
+      </c>
+      <c r="I9">
+        <v>2030</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9">
+        <v>-0.5</v>
+      </c>
+      <c r="M9" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC300CF1-742B-4AF3-AFD8-3A05A0033F3F}">
+  <sheetPr>
+    <tabColor theme="8"/>
+  </sheetPr>
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.28515625" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="9">
+        <v>0.35299999999999998</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15">
+      <c r="B2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="9">
+        <v>9.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15">
+      <c r="B3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="9">
+        <f>E1-E2</f>
+        <v>0.25800000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="15">
+      <c r="J4" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="B5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="B6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6">
+        <v>3</v>
+      </c>
+      <c r="L6">
+        <v>3</v>
+      </c>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="B7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7">
+        <v>3</v>
+      </c>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="B8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="2" t="str">
+        <f>D6</f>
+        <v>ET*,-ETRAN*</v>
+      </c>
+      <c r="I8">
+        <v>2017</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="B9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="2" t="str">
+        <f>D7</f>
+        <v>ERW*</v>
+      </c>
+      <c r="I9">
+        <v>2017</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9">
+        <f>-E3*10%</f>
+        <v>-2.5800000000000003E-2</v>
+      </c>
+      <c r="M9" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{094F3F01-6F8D-4CDF-BA87-A82A1DC1CDCE}">
+  <sheetPr>
+    <tabColor theme="8"/>
+  </sheetPr>
+  <dimension ref="A1:N14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" customWidth="1"/>
+    <col min="10" max="10" width="16" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1">
+        <v>2026</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="15">
+      <c r="B2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="15">
+      <c r="B3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="9"/>
+    </row>
+    <row r="4" spans="1:14" ht="15">
+      <c r="G4" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="B5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" s="11" t="str">
+        <f>"UC_RHSRT~"&amp;G1</f>
+        <v>UC_RHSRT~2026</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="B6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6">
+        <f>G1</f>
+        <v>2026</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6">
+        <f>1+$E$1</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <f>-E2</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="2">
         <v>5</v>
       </c>
-      <c r="M8" s="2" t="s">
+    </row>
+    <row r="7" spans="1:14">
+      <c r="B7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7">
+        <v>2054</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7">
+        <f>1+$E$1</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H7">
         <v>1</v>
       </c>
+      <c r="I7">
+        <f>-E3</f>
+        <v>0</v>
+      </c>
+      <c r="J7" s="2">
+        <v>5</v>
+      </c>
     </row>
-    <row r="9" spans="1:13" ht="15">
+    <row r="8" spans="1:14">
+      <c r="B8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8">
+        <v>2055</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8">
+        <v>100</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <f>-E3</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="B9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>2</v>
+        <v>42</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9">
+        <f>E6</f>
+        <v>2026</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9">
+        <f>G6</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
       </c>
       <c r="I9">
-        <v>2050</v>
-      </c>
-      <c r="J9" t="s">
+        <f>-E3</f>
         <v>0</v>
       </c>
-      <c r="K9">
+      <c r="J9" s="2">
+        <v>5</v>
+      </c>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="B10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10">
+        <f>E7</f>
+        <v>2054</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10">
+        <f>G7</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H10">
         <v>1</v>
       </c>
-      <c r="L9">
+      <c r="I10">
+        <f>-E3</f>
+        <v>0</v>
+      </c>
+      <c r="J10" s="2">
+        <v>5</v>
+      </c>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="B11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11">
+        <f t="shared" ref="E11:E14" si="0">E8</f>
+        <v>2055</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11">
+        <f t="shared" ref="G11:G14" si="1">G8</f>
         <v>100</v>
       </c>
-      <c r="M9" s="2" t="s">
+      <c r="H11">
         <v>1</v>
+      </c>
+      <c r="I11">
+        <f>-E4</f>
+        <v>0</v>
+      </c>
+      <c r="J11" s="2">
+        <v>5</v>
+      </c>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="B12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>2026</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12">
+        <v>1.5</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12" s="2">
+        <v>5</v>
+      </c>
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="B13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>2054</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13">
+        <v>1.5</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="B14" s="2" t="str">
+        <f>B12</f>
+        <v>UC_Growth_Batteries</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="2" t="str">
+        <f>D12</f>
+        <v>ESTSUTL</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>2055</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14" s="2">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UC growth added to Nuclear and on the demand side
</commit_message>
<xml_diff>
--- a/suppxls/Scen_UC_ELC.xlsx
+++ b/suppxls/Scen_UC_ELC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\suppxls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51FE3693-826C-454E-B3BE-DB87769AC88C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFAB8FAA-BC46-4CAE-B2BB-83E12F661B6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1890" yWindow="1170" windowWidth="26610" windowHeight="13740" firstSheet="1" activeTab="4" xr2:uid="{22D7DAD2-FC1B-44BE-801D-D5E60FB61EEE}"/>
+    <workbookView xWindow="1290" yWindow="870" windowWidth="26610" windowHeight="13740" firstSheet="5" activeTab="8" xr2:uid="{22D7DAD2-FC1B-44BE-801D-D5E60FB61EEE}"/>
   </bookViews>
   <sheets>
     <sheet name="BuildRateConstraints" sheetId="1" r:id="rId1"/>
@@ -19,11 +19,11 @@
     <sheet name="FIRMConstraint" sheetId="3" r:id="rId4"/>
     <sheet name="WindPVConstraint" sheetId="8" r:id="rId5"/>
     <sheet name="WindThermalConstraint" sheetId="6" r:id="rId6"/>
-    <sheet name="GrowthConstraints" sheetId="7" r:id="rId7"/>
+    <sheet name="GrowthConstraintsSupply" sheetId="7" r:id="rId7"/>
+    <sheet name="GrowthConstraintsDistribution" sheetId="9" r:id="rId8"/>
+    <sheet name="GrowthConstraintsTransport" sheetId="10" r:id="rId9"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId8"/>
-    <externalReference r:id="rId9"/>
     <externalReference r:id="rId10"/>
     <externalReference r:id="rId11"/>
     <externalReference r:id="rId12"/>
@@ -36,6 +36,8 @@
     <externalReference r:id="rId19"/>
     <externalReference r:id="rId20"/>
     <externalReference r:id="rId21"/>
+    <externalReference r:id="rId22"/>
+    <externalReference r:id="rId23"/>
   </externalReferences>
   <definedNames>
     <definedName name="\I">#REF!</definedName>
@@ -1833,7 +1835,9 @@
     <definedName name="LOADFACTOR3">#REF!</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="2" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="3" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="7" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="6" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="8" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="1" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="4" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="5" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -2017,7 +2021,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="66">
   <si>
     <t>UP</t>
   </si>
@@ -2161,6 +2165,60 @@
   </si>
   <si>
     <t>Year Start</t>
+  </si>
+  <si>
+    <t>ACT,GROWTH</t>
+  </si>
+  <si>
+    <t>Starting Value ELC</t>
+  </si>
+  <si>
+    <t>Starting Value HGN</t>
+  </si>
+  <si>
+    <t>UC_ACT~RHS</t>
+  </si>
+  <si>
+    <t>XINDELC</t>
+  </si>
+  <si>
+    <t>XINDHGN</t>
+  </si>
+  <si>
+    <t>UC_Growth_Nuclear</t>
+  </si>
+  <si>
+    <t>ETNUC*N</t>
+  </si>
+  <si>
+    <t>XICPELC</t>
+  </si>
+  <si>
+    <t>XIMIELC</t>
+  </si>
+  <si>
+    <t>XIFBELC</t>
+  </si>
+  <si>
+    <t>XTRAELC</t>
+  </si>
+  <si>
+    <t>TPPRCARELC-N</t>
+  </si>
+  <si>
+    <t>Starting Value</t>
+  </si>
+  <si>
+    <t>TFLCVELC-N</t>
+  </si>
+  <si>
+    <t>TFHCV1ELC-N</t>
+  </si>
+  <si>
+    <t>TPPUMBTELC-N</t>
+  </si>
+  <si>
+    <t>TFLCVOGSH-N</t>
   </si>
 </sst>
 </file>
@@ -20551,7 +20609,7 @@
   </sheetPr>
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
@@ -20899,10 +20957,10 @@
   <sheetPr>
     <tabColor theme="8"/>
   </sheetPr>
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -21159,7 +21217,7 @@
         <v>41</v>
       </c>
       <c r="E11">
-        <f t="shared" ref="E11:E14" si="0">E8</f>
+        <f t="shared" ref="E11:E17" si="0">E8</f>
         <v>2055</v>
       </c>
       <c r="F11" s="2" t="s">
@@ -21275,6 +21333,1441 @@
         <v>5</v>
       </c>
     </row>
+    <row r="15" spans="1:14">
+      <c r="B15" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>2026</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>-1</v>
+      </c>
+      <c r="J15" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="B16" s="2" t="str">
+        <f>B15</f>
+        <v>UC_Growth_Nuclear</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="2" t="str">
+        <f>D15</f>
+        <v>ETNUC*N</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>2054</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <f>I15</f>
+        <v>-1</v>
+      </c>
+      <c r="J16" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10">
+      <c r="B17" s="2" t="str">
+        <f>B15</f>
+        <v>UC_Growth_Nuclear</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="2" t="str">
+        <f>D15</f>
+        <v>ETNUC*N</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>2055</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17">
+        <f t="shared" ref="G17" si="2">G14</f>
+        <v>100</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <f>I16</f>
+        <v>-1</v>
+      </c>
+      <c r="J17" s="2">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51E68AFE-4568-41C3-A0A2-B498ECB4C44C}">
+  <sheetPr>
+    <tabColor theme="8"/>
+  </sheetPr>
+  <dimension ref="A1:N26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" customWidth="1"/>
+    <col min="10" max="10" width="16" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1">
+        <v>2026</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15">
+      <c r="B2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15">
+      <c r="B3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15">
+      <c r="G4" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="B5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5" s="11" t="str">
+        <f>"UC_RHSRT~"&amp;G1</f>
+        <v>UC_RHSRT~2026</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="B6" s="2" t="str">
+        <f>"UC_Growth_"&amp;D6</f>
+        <v>UC_Growth_XINDELC</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6">
+        <f>G1</f>
+        <v>2026</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6">
+        <f>1+$E$1</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <f>-E2</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="B7" s="2" t="str">
+        <f t="shared" ref="B7:B8" si="0">"UC_Growth_"&amp;D7</f>
+        <v>UC_Growth_XINDELC</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="2" t="str">
+        <f>D6</f>
+        <v>XINDELC</v>
+      </c>
+      <c r="E7">
+        <v>2054</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7">
+        <f>1+$E$1</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <f>I6</f>
+        <v>0</v>
+      </c>
+      <c r="J7" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="B8" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>UC_Growth_XINDELC</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="2" t="str">
+        <f>D7</f>
+        <v>XINDELC</v>
+      </c>
+      <c r="E8">
+        <v>2055</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8">
+        <v>100</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <f>I7</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="B9" s="2" t="str">
+        <f>"UC_Growth_"&amp;D9</f>
+        <v>UC_Growth_XICPELC</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9">
+        <f>E6</f>
+        <v>2026</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9">
+        <f>1+$E$1</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <f>I6</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="B10" s="2" t="str">
+        <f t="shared" ref="B10:B11" si="1">"UC_Growth_"&amp;D10</f>
+        <v>UC_Growth_XICPELC</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="2" t="str">
+        <f>D9</f>
+        <v>XICPELC</v>
+      </c>
+      <c r="E10">
+        <f t="shared" ref="E10:E20" si="2">E7</f>
+        <v>2054</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10">
+        <f>1+$E$1</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <f t="shared" ref="I10:I20" si="3">I7</f>
+        <v>0</v>
+      </c>
+      <c r="J10" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="B11" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>UC_Growth_XICPELC</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="2" t="str">
+        <f>D10</f>
+        <v>XICPELC</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="2"/>
+        <v>2055</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11">
+        <v>100</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="B12" s="2" t="str">
+        <f>"UC_Growth_"&amp;D12</f>
+        <v>UC_Growth_XIMIELC</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="2"/>
+        <v>2026</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12">
+        <f>1+$E$1</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="B13" s="2" t="str">
+        <f t="shared" ref="B13:B14" si="4">"UC_Growth_"&amp;D13</f>
+        <v>UC_Growth_XIMIELC</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="2" t="str">
+        <f>D12</f>
+        <v>XIMIELC</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="2"/>
+        <v>2054</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13">
+        <f>1+$E$1</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="B14" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>UC_Growth_XIMIELC</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="2" t="str">
+        <f>D13</f>
+        <v>XIMIELC</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="2"/>
+        <v>2055</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14">
+        <v>100</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="B15" s="2" t="str">
+        <f>"UC_Growth_"&amp;D15</f>
+        <v>UC_Growth_XIFBELC</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="2"/>
+        <v>2026</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15">
+        <f>1+$E$1</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="B16" s="2" t="str">
+        <f t="shared" ref="B16:B17" si="5">"UC_Growth_"&amp;D16</f>
+        <v>UC_Growth_XIFBELC</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="2" t="str">
+        <f>D15</f>
+        <v>XIFBELC</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="2"/>
+        <v>2054</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16">
+        <f>1+$E$1</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14">
+      <c r="B17" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>UC_Growth_XIFBELC</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="2" t="str">
+        <f>D16</f>
+        <v>XIFBELC</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="2"/>
+        <v>2055</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17">
+        <v>100</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14">
+      <c r="B18" s="2" t="str">
+        <f>"UC_Growth_"&amp;D18</f>
+        <v>UC_Growth_XTRAELC</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>2026</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18">
+        <f>1+$E$1</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J18" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14">
+      <c r="B19" s="2" t="str">
+        <f t="shared" ref="B19:B20" si="6">"UC_Growth_"&amp;D19</f>
+        <v>UC_Growth_XTRAELC</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="2" t="str">
+        <f>D18</f>
+        <v>XTRAELC</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>2054</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19">
+        <f>1+$E$1</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J19" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14">
+      <c r="B20" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>UC_Growth_XTRAELC</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="2" t="str">
+        <f>D19</f>
+        <v>XTRAELC</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="2"/>
+        <v>2055</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20">
+        <v>100</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J20" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14">
+      <c r="B21" s="2" t="str">
+        <f>"UC_Growth_"&amp;D21</f>
+        <v>UC_Growth_XINDHGN</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21">
+        <f>E15</f>
+        <v>2026</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21">
+        <f>1+$E$1</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <f>I15</f>
+        <v>0</v>
+      </c>
+      <c r="J21" s="2">
+        <v>5</v>
+      </c>
+      <c r="N21" s="2"/>
+    </row>
+    <row r="22" spans="2:14">
+      <c r="B22" s="2" t="str">
+        <f t="shared" ref="B22:B23" si="7">"UC_Growth_"&amp;D22</f>
+        <v>UC_Growth_XINDHGN</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22">
+        <f>E16</f>
+        <v>2054</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22">
+        <f>1+$E$1</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <f>I16</f>
+        <v>0</v>
+      </c>
+      <c r="J22" s="2">
+        <v>5</v>
+      </c>
+      <c r="N22" s="2"/>
+    </row>
+    <row r="23" spans="2:14">
+      <c r="B23" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>UC_Growth_XINDHGN</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23">
+        <f>E17</f>
+        <v>2055</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G23">
+        <v>100</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <f>I17</f>
+        <v>0</v>
+      </c>
+      <c r="J23" s="2">
+        <v>5</v>
+      </c>
+      <c r="N23" s="2"/>
+    </row>
+    <row r="24" spans="2:14">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="N24" s="2"/>
+    </row>
+    <row r="25" spans="2:14">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="J25" s="2"/>
+    </row>
+    <row r="26" spans="2:14">
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="J26" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BF23F5D-A00A-4460-8453-94D06916B235}">
+  <sheetPr>
+    <tabColor theme="8"/>
+  </sheetPr>
+  <dimension ref="A1:N20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" customWidth="1"/>
+    <col min="10" max="10" width="16" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="15">
+      <c r="B2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="15">
+      <c r="B3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:14" ht="15">
+      <c r="G4" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="B5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" s="11" t="str">
+        <f>"UC_RHSRT~"&amp;G1</f>
+        <v>UC_RHSRT~2024</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="B6" s="2" t="str">
+        <f>"UC_Growth_"&amp;D6</f>
+        <v>UC_Growth_TPPRCARELC-N</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6">
+        <f>G1</f>
+        <v>2024</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6">
+        <f>1+$E$1</f>
+        <v>1.2</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <f>-E2</f>
+        <v>-10</v>
+      </c>
+      <c r="J6" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="B7" s="2" t="str">
+        <f t="shared" ref="B7:B14" si="0">"UC_Growth_"&amp;D7</f>
+        <v>UC_Growth_TPPRCARELC-N</v>
+      </c>
+      <c r="C7" s="2" t="str">
+        <f>C6</f>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D7" s="2" t="str">
+        <f>D6</f>
+        <v>TPPRCARELC-N</v>
+      </c>
+      <c r="E7">
+        <v>2054</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7">
+        <f>1+$E$1</f>
+        <v>1.2</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <f>I6</f>
+        <v>-10</v>
+      </c>
+      <c r="J7" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="B8" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>UC_Growth_TPPRCARELC-N</v>
+      </c>
+      <c r="C8" s="2" t="str">
+        <f>C7</f>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D8" s="2" t="str">
+        <f>D7</f>
+        <v>TPPRCARELC-N</v>
+      </c>
+      <c r="E8">
+        <v>2055</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8">
+        <v>100</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <f>I7</f>
+        <v>-10</v>
+      </c>
+      <c r="J8" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="B9" s="2" t="str">
+        <f>"UC_Growth_"&amp;D9</f>
+        <v>UC_Growth_TPPUMBTELC-N</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9">
+        <f>$G$1</f>
+        <v>2024</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9">
+        <f>1+$E$1</f>
+        <v>1.2</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>-2</v>
+      </c>
+      <c r="J9" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="B10" s="2" t="str">
+        <f t="shared" ref="B10:B11" si="1">"UC_Growth_"&amp;D10</f>
+        <v>UC_Growth_TPPUMBTELC-N</v>
+      </c>
+      <c r="C10" s="2" t="str">
+        <f>C9</f>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D10" s="2" t="str">
+        <f>D9</f>
+        <v>TPPUMBTELC-N</v>
+      </c>
+      <c r="E10">
+        <v>2054</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10">
+        <f>1+$E$1</f>
+        <v>1.2</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <f>I9</f>
+        <v>-2</v>
+      </c>
+      <c r="J10" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="B11" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>UC_Growth_TPPUMBTELC-N</v>
+      </c>
+      <c r="C11" s="2" t="str">
+        <f>C10</f>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D11" s="2" t="str">
+        <f>D10</f>
+        <v>TPPUMBTELC-N</v>
+      </c>
+      <c r="E11">
+        <v>2055</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11">
+        <v>100</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <f>I10</f>
+        <v>-2</v>
+      </c>
+      <c r="J11" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="B12" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>UC_Growth_TFLCVOGSH-N</v>
+      </c>
+      <c r="C12" s="2" t="str">
+        <f>C8</f>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12">
+        <f>E6</f>
+        <v>2024</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12">
+        <f>1+$E$1</f>
+        <v>1.2</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <f>-$E$2</f>
+        <v>-10</v>
+      </c>
+      <c r="J12" s="2">
+        <v>5</v>
+      </c>
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="B13" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>UC_Growth_TFLCVOGSH-N</v>
+      </c>
+      <c r="C13" s="2" t="str">
+        <f t="shared" ref="C13:C17" si="2">C12</f>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D13" s="2" t="str">
+        <f>D12</f>
+        <v>TFLCVOGSH-N</v>
+      </c>
+      <c r="E13">
+        <f>E7</f>
+        <v>2054</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13">
+        <f>1+$E$1</f>
+        <v>1.2</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <f>I12</f>
+        <v>-10</v>
+      </c>
+      <c r="J13" s="2">
+        <v>5</v>
+      </c>
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="B14" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>UC_Growth_TFLCVOGSH-N</v>
+      </c>
+      <c r="C14" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D14" s="2" t="str">
+        <f>D13</f>
+        <v>TFLCVOGSH-N</v>
+      </c>
+      <c r="E14">
+        <f>E8</f>
+        <v>2055</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14">
+        <v>100</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <f>I13</f>
+        <v>-10</v>
+      </c>
+      <c r="J14" s="2">
+        <v>5</v>
+      </c>
+      <c r="N14" s="2"/>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="B15" s="2" t="str">
+        <f t="shared" ref="B15:B17" si="3">"UC_Growth_"&amp;D15</f>
+        <v>UC_Growth_TFLCVELC-N</v>
+      </c>
+      <c r="C15" s="2" t="str">
+        <f>C11</f>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15">
+        <f>E9</f>
+        <v>2024</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15">
+        <f>1+$E$1</f>
+        <v>1.2</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <f>-$E$2</f>
+        <v>-10</v>
+      </c>
+      <c r="J15" s="2">
+        <v>5</v>
+      </c>
+      <c r="N15" s="2"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="B16" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>UC_Growth_TFLCVELC-N</v>
+      </c>
+      <c r="C16" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D16" s="2" t="str">
+        <f>D15</f>
+        <v>TFLCVELC-N</v>
+      </c>
+      <c r="E16">
+        <f>E10</f>
+        <v>2054</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16">
+        <f>1+$E$1</f>
+        <v>1.2</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <f>I15</f>
+        <v>-10</v>
+      </c>
+      <c r="J16" s="2">
+        <v>5</v>
+      </c>
+      <c r="N16" s="2"/>
+    </row>
+    <row r="17" spans="2:14">
+      <c r="B17" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>UC_Growth_TFLCVELC-N</v>
+      </c>
+      <c r="C17" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D17" s="2" t="str">
+        <f>D16</f>
+        <v>TFLCVELC-N</v>
+      </c>
+      <c r="E17">
+        <f>E11</f>
+        <v>2055</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17">
+        <v>100</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <f>I16</f>
+        <v>-10</v>
+      </c>
+      <c r="J17" s="2">
+        <v>5</v>
+      </c>
+      <c r="N17" s="2"/>
+    </row>
+    <row r="18" spans="2:14">
+      <c r="B18" s="2" t="str">
+        <f t="shared" ref="B18:B20" si="4">"UC_Growth_"&amp;D18</f>
+        <v>UC_Growth_TFHCV1ELC-N</v>
+      </c>
+      <c r="C18" s="2" t="str">
+        <f>C14</f>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18">
+        <f>E12</f>
+        <v>2024</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18">
+        <f>1+$E$1</f>
+        <v>1.2</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>-5</v>
+      </c>
+      <c r="J18" s="2">
+        <v>5</v>
+      </c>
+      <c r="N18" s="2"/>
+    </row>
+    <row r="19" spans="2:14">
+      <c r="B19" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>UC_Growth_TFHCV1ELC-N</v>
+      </c>
+      <c r="C19" s="2" t="str">
+        <f t="shared" ref="C19:C20" si="5">C18</f>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D19" s="2" t="str">
+        <f>D18</f>
+        <v>TFHCV1ELC-N</v>
+      </c>
+      <c r="E19">
+        <f>E13</f>
+        <v>2054</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19">
+        <f>1+$E$1</f>
+        <v>1.2</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <f>I18</f>
+        <v>-5</v>
+      </c>
+      <c r="J19" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14">
+      <c r="B20" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>UC_Growth_TFHCV1ELC-N</v>
+      </c>
+      <c r="C20" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D20" s="2" t="str">
+        <f>D19</f>
+        <v>TFHCV1ELC-N</v>
+      </c>
+      <c r="E20">
+        <f>E14</f>
+        <v>2055</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20">
+        <v>100</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <f>I19</f>
+        <v>-5</v>
+      </c>
+      <c r="J20" s="2">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Growth constraints added to other vehicles
</commit_message>
<xml_diff>
--- a/suppxls/Scen_UC_ELC.xlsx
+++ b/suppxls/Scen_UC_ELC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\suppxls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFAB8FAA-BC46-4CAE-B2BB-83E12F661B6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAD9FDF7-2F13-4E65-AB58-4B7B4543EB65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1290" yWindow="870" windowWidth="26610" windowHeight="13740" firstSheet="5" activeTab="8" xr2:uid="{22D7DAD2-FC1B-44BE-801D-D5E60FB61EEE}"/>
+    <workbookView xWindow="1230" yWindow="975" windowWidth="26610" windowHeight="13740" firstSheet="5" activeTab="8" xr2:uid="{22D7DAD2-FC1B-44BE-801D-D5E60FB61EEE}"/>
   </bookViews>
   <sheets>
     <sheet name="BuildRateConstraints" sheetId="1" r:id="rId1"/>
@@ -21440,10 +21440,10 @@
   <sheetPr>
     <tabColor theme="8"/>
   </sheetPr>
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -21678,7 +21678,7 @@
         <v>XICPELC</v>
       </c>
       <c r="E10">
-        <f t="shared" ref="E10:E20" si="2">E7</f>
+        <f t="shared" ref="E10:E17" si="2">E7</f>
         <v>2054</v>
       </c>
       <c r="F10" s="2" t="s">
@@ -21692,7 +21692,7 @@
         <v>1</v>
       </c>
       <c r="I10">
-        <f t="shared" ref="I10:I20" si="3">I7</f>
+        <f t="shared" ref="I10:I17" si="3">I7</f>
         <v>0</v>
       </c>
       <c r="J10" s="2">
@@ -21935,16 +21935,16 @@
     <row r="18" spans="2:14">
       <c r="B18" s="2" t="str">
         <f>"UC_Growth_"&amp;D18</f>
-        <v>UC_Growth_XTRAELC</v>
+        <v>UC_Growth_XINDHGN</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E18">
-        <f t="shared" si="2"/>
+        <f>E15</f>
         <v>2026</v>
       </c>
       <c r="F18" s="2" t="s">
@@ -21958,7 +21958,7 @@
         <v>1</v>
       </c>
       <c r="I18">
-        <f t="shared" si="3"/>
+        <f>I15</f>
         <v>0</v>
       </c>
       <c r="J18" s="2">
@@ -21968,17 +21968,16 @@
     <row r="19" spans="2:14">
       <c r="B19" s="2" t="str">
         <f t="shared" ref="B19:B20" si="6">"UC_Growth_"&amp;D19</f>
-        <v>UC_Growth_XTRAELC</v>
+        <v>UC_Growth_XINDHGN</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="2" t="str">
-        <f>D18</f>
-        <v>XTRAELC</v>
+      <c r="D19" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="E19">
-        <f t="shared" si="2"/>
+        <f>E16</f>
         <v>2054</v>
       </c>
       <c r="F19" s="2" t="s">
@@ -21992,7 +21991,7 @@
         <v>1</v>
       </c>
       <c r="I19">
-        <f t="shared" si="3"/>
+        <f>I16</f>
         <v>0</v>
       </c>
       <c r="J19" s="2">
@@ -22002,17 +22001,16 @@
     <row r="20" spans="2:14">
       <c r="B20" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>UC_Growth_XTRAELC</v>
+        <v>UC_Growth_XINDHGN</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="2" t="str">
-        <f>D19</f>
-        <v>XTRAELC</v>
+      <c r="D20" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="E20">
-        <f t="shared" si="2"/>
+        <f>E17</f>
         <v>2055</v>
       </c>
       <c r="F20" s="2" t="s">
@@ -22025,7 +22023,7 @@
         <v>1</v>
       </c>
       <c r="I20">
-        <f t="shared" si="3"/>
+        <f>I17</f>
         <v>0</v>
       </c>
       <c r="J20" s="2">
@@ -22035,13 +22033,13 @@
     <row r="21" spans="2:14">
       <c r="B21" s="2" t="str">
         <f>"UC_Growth_"&amp;D21</f>
-        <v>UC_Growth_XINDHGN</v>
+        <v>UC_Growth_XTRAELC</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="E21">
         <f>E15</f>
@@ -22069,13 +22067,14 @@
     <row r="22" spans="2:14">
       <c r="B22" s="2" t="str">
         <f t="shared" ref="B22:B23" si="7">"UC_Growth_"&amp;D22</f>
-        <v>UC_Growth_XINDHGN</v>
+        <v>UC_Growth_XTRAELC</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>53</v>
+      <c r="D22" s="2" t="str">
+        <f>D21</f>
+        <v>XTRAELC</v>
       </c>
       <c r="E22">
         <f>E16</f>
@@ -22103,13 +22102,14 @@
     <row r="23" spans="2:14">
       <c r="B23" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>UC_Growth_XINDHGN</v>
+        <v>UC_Growth_XTRAELC</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>53</v>
+      <c r="D23" s="2" t="str">
+        <f>D22</f>
+        <v>XTRAELC</v>
       </c>
       <c r="E23">
         <f>E17</f>
@@ -22134,26 +22134,7 @@
       <c r="N23" s="2"/>
     </row>
     <row r="24" spans="2:14">
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="J24" s="2"/>
       <c r="N24" s="2"/>
-    </row>
-    <row r="25" spans="2:14">
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="J25" s="2"/>
-    </row>
-    <row r="26" spans="2:14">
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="J26" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -22168,7 +22149,7 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -22466,7 +22447,7 @@
         <v>65</v>
       </c>
       <c r="E12">
-        <f>E6</f>
+        <f t="shared" ref="E12:E20" si="2">E6</f>
         <v>2024</v>
       </c>
       <c r="F12" s="2" t="s">
@@ -22494,7 +22475,7 @@
         <v>UC_Growth_TFLCVOGSH-N</v>
       </c>
       <c r="C13" s="2" t="str">
-        <f t="shared" ref="C13:C17" si="2">C12</f>
+        <f t="shared" ref="C13:C17" si="3">C12</f>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D13" s="2" t="str">
@@ -22502,7 +22483,7 @@
         <v>TFLCVOGSH-N</v>
       </c>
       <c r="E13">
-        <f>E7</f>
+        <f t="shared" si="2"/>
         <v>2054</v>
       </c>
       <c r="F13" s="2" t="s">
@@ -22530,7 +22511,7 @@
         <v>UC_Growth_TFLCVOGSH-N</v>
       </c>
       <c r="C14" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D14" s="2" t="str">
@@ -22538,7 +22519,7 @@
         <v>TFLCVOGSH-N</v>
       </c>
       <c r="E14">
-        <f>E8</f>
+        <f t="shared" si="2"/>
         <v>2055</v>
       </c>
       <c r="F14" s="2" t="s">
@@ -22561,7 +22542,7 @@
     </row>
     <row r="15" spans="1:14">
       <c r="B15" s="2" t="str">
-        <f t="shared" ref="B15:B17" si="3">"UC_Growth_"&amp;D15</f>
+        <f t="shared" ref="B15:B17" si="4">"UC_Growth_"&amp;D15</f>
         <v>UC_Growth_TFLCVELC-N</v>
       </c>
       <c r="C15" s="2" t="str">
@@ -22572,7 +22553,7 @@
         <v>62</v>
       </c>
       <c r="E15">
-        <f>E9</f>
+        <f t="shared" si="2"/>
         <v>2024</v>
       </c>
       <c r="F15" s="2" t="s">
@@ -22596,11 +22577,11 @@
     </row>
     <row r="16" spans="1:14">
       <c r="B16" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>UC_Growth_TFLCVELC-N</v>
+      </c>
+      <c r="C16" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>UC_Growth_TFLCVELC-N</v>
-      </c>
-      <c r="C16" s="2" t="str">
-        <f t="shared" si="2"/>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D16" s="2" t="str">
@@ -22608,7 +22589,7 @@
         <v>TFLCVELC-N</v>
       </c>
       <c r="E16">
-        <f>E10</f>
+        <f t="shared" si="2"/>
         <v>2054</v>
       </c>
       <c r="F16" s="2" t="s">
@@ -22632,11 +22613,11 @@
     </row>
     <row r="17" spans="2:14">
       <c r="B17" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>UC_Growth_TFLCVELC-N</v>
+      </c>
+      <c r="C17" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>UC_Growth_TFLCVELC-N</v>
-      </c>
-      <c r="C17" s="2" t="str">
-        <f t="shared" si="2"/>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D17" s="2" t="str">
@@ -22644,7 +22625,7 @@
         <v>TFLCVELC-N</v>
       </c>
       <c r="E17">
-        <f>E11</f>
+        <f t="shared" si="2"/>
         <v>2055</v>
       </c>
       <c r="F17" s="2" t="s">
@@ -22667,7 +22648,7 @@
     </row>
     <row r="18" spans="2:14">
       <c r="B18" s="2" t="str">
-        <f t="shared" ref="B18:B20" si="4">"UC_Growth_"&amp;D18</f>
+        <f t="shared" ref="B18:B20" si="5">"UC_Growth_"&amp;D18</f>
         <v>UC_Growth_TFHCV1ELC-N</v>
       </c>
       <c r="C18" s="2" t="str">
@@ -22678,7 +22659,7 @@
         <v>63</v>
       </c>
       <c r="E18">
-        <f>E12</f>
+        <f t="shared" si="2"/>
         <v>2024</v>
       </c>
       <c r="F18" s="2" t="s">
@@ -22701,11 +22682,11 @@
     </row>
     <row r="19" spans="2:14">
       <c r="B19" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>UC_Growth_TFHCV1ELC-N</v>
       </c>
       <c r="C19" s="2" t="str">
-        <f t="shared" ref="C19:C20" si="5">C18</f>
+        <f t="shared" ref="C19:C20" si="6">C18</f>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D19" s="2" t="str">
@@ -22713,7 +22694,7 @@
         <v>TFHCV1ELC-N</v>
       </c>
       <c r="E19">
-        <f>E13</f>
+        <f t="shared" si="2"/>
         <v>2054</v>
       </c>
       <c r="F19" s="2" t="s">
@@ -22736,11 +22717,11 @@
     </row>
     <row r="20" spans="2:14">
       <c r="B20" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>UC_Growth_TFHCV1ELC-N</v>
       </c>
       <c r="C20" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D20" s="2" t="str">
@@ -22748,7 +22729,7 @@
         <v>TFHCV1ELC-N</v>
       </c>
       <c r="E20">
-        <f>E14</f>
+        <f t="shared" si="2"/>
         <v>2055</v>
       </c>
       <c r="F20" s="2" t="s">

</xml_diff>

<commit_message>
TRA, UCGrowth and SHAPE updated doing last fixes on transport
</commit_message>
<xml_diff>
--- a/suppxls/Scen_UC_ELC.xlsx
+++ b/suppxls/Scen_UC_ELC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\suppxls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAD9FDF7-2F13-4E65-AB58-4B7B4543EB65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0901D2C-3FC3-4C47-9E5A-2EE9D305F3B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1230" yWindow="975" windowWidth="26610" windowHeight="13740" firstSheet="5" activeTab="8" xr2:uid="{22D7DAD2-FC1B-44BE-801D-D5E60FB61EEE}"/>
+    <workbookView xWindow="4065" yWindow="-19140" windowWidth="26610" windowHeight="13740" firstSheet="5" activeTab="8" xr2:uid="{22D7DAD2-FC1B-44BE-801D-D5E60FB61EEE}"/>
   </bookViews>
   <sheets>
     <sheet name="BuildRateConstraints" sheetId="1" r:id="rId1"/>
@@ -2021,7 +2021,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="81">
   <si>
     <t>UP</t>
   </si>
@@ -2219,6 +2219,51 @@
   </si>
   <si>
     <t>TFLCVOGSH-N</t>
+  </si>
+  <si>
+    <t>TPPRCARHGNF-N</t>
+  </si>
+  <si>
+    <t>TPPRSUVELC-N</t>
+  </si>
+  <si>
+    <t>TPPRSUVHGNF-N</t>
+  </si>
+  <si>
+    <t>TFHCV2ELC-N</t>
+  </si>
+  <si>
+    <t>TFHCV3ELC-N</t>
+  </si>
+  <si>
+    <t>TFHCV4ELC-N</t>
+  </si>
+  <si>
+    <t>TFHCV5ELC-N</t>
+  </si>
+  <si>
+    <t>TFHCV6ELC-N</t>
+  </si>
+  <si>
+    <t>TFHCV7ELC-N</t>
+  </si>
+  <si>
+    <t>TFHCV2HGN-N</t>
+  </si>
+  <si>
+    <t>TFHCV3HGN-N</t>
+  </si>
+  <si>
+    <t>TFHCV4HGN-N</t>
+  </si>
+  <si>
+    <t>TFHCV5HGN-N</t>
+  </si>
+  <si>
+    <t>TFHCV6HGN-N</t>
+  </si>
+  <si>
+    <t>TFHCV7HGN-N</t>
   </si>
 </sst>
 </file>
@@ -22146,15 +22191,15 @@
   <sheetPr>
     <tabColor theme="8"/>
   </sheetPr>
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:N68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="B71" sqref="B71:B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" customWidth="1"/>
     <col min="4" max="4" width="23.5703125" customWidth="1"/>
     <col min="8" max="8" width="16.85546875" customWidth="1"/>
@@ -22163,7 +22208,7 @@
     <col min="13" max="13" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -22180,7 +22225,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15">
+    <row r="2" spans="1:11" ht="15">
       <c r="B2" s="7" t="s">
         <v>18</v>
       </c>
@@ -22191,18 +22236,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15">
+    <row r="3" spans="1:11" ht="15">
       <c r="B3" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:14" ht="15">
+    <row r="4" spans="1:11" ht="15">
       <c r="G4" s="8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:11">
       <c r="B5" s="6" t="s">
         <v>15</v>
       </c>
@@ -22235,7 +22280,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:11">
       <c r="B6" s="2" t="str">
         <f>"UC_Growth_"&amp;D6</f>
         <v>UC_Growth_TPPRCARELC-N</v>
@@ -22261,16 +22306,16 @@
         <v>1</v>
       </c>
       <c r="I6">
-        <f>-E2</f>
+        <f>-$E$2</f>
         <v>-10</v>
       </c>
       <c r="J6" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:11">
       <c r="B7" s="2" t="str">
-        <f t="shared" ref="B7:B14" si="0">"UC_Growth_"&amp;D7</f>
+        <f t="shared" ref="B7:B23" si="0">"UC_Growth_"&amp;D7</f>
         <v>UC_Growth_TPPRCARELC-N</v>
       </c>
       <c r="C7" s="2" t="str">
@@ -22302,7 +22347,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:11">
       <c r="B8" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_Growth_TPPRCARELC-N</v>
@@ -22335,19 +22380,19 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:11">
       <c r="B9" s="2" t="str">
         <f>"UC_Growth_"&amp;D9</f>
-        <v>UC_Growth_TPPUMBTELC-N</v>
+        <v>UC_Growth_TPPRCARHGNF-N</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E9">
-        <f>$G$1</f>
+        <f>E6</f>
         <v>2024</v>
       </c>
       <c r="F9" s="2" t="s">
@@ -22361,16 +22406,17 @@
         <v>1</v>
       </c>
       <c r="I9">
-        <v>-2</v>
+        <f>-$E$2</f>
+        <v>-10</v>
       </c>
       <c r="J9" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:11">
       <c r="B10" s="2" t="str">
         <f t="shared" ref="B10:B11" si="1">"UC_Growth_"&amp;D10</f>
-        <v>UC_Growth_TPPUMBTELC-N</v>
+        <v>UC_Growth_TPPRCARHGNF-N</v>
       </c>
       <c r="C10" s="2" t="str">
         <f>C9</f>
@@ -22378,7 +22424,7 @@
       </c>
       <c r="D10" s="2" t="str">
         <f>D9</f>
-        <v>TPPUMBTELC-N</v>
+        <v>TPPRCARHGNF-N</v>
       </c>
       <c r="E10">
         <v>2054</v>
@@ -22395,16 +22441,16 @@
       </c>
       <c r="I10">
         <f>I9</f>
-        <v>-2</v>
+        <v>-10</v>
       </c>
       <c r="J10" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:11">
       <c r="B11" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>UC_Growth_TPPUMBTELC-N</v>
+        <v>UC_Growth_TPPRCARHGNF-N</v>
       </c>
       <c r="C11" s="2" t="str">
         <f>C10</f>
@@ -22412,7 +22458,7 @@
       </c>
       <c r="D11" s="2" t="str">
         <f>D10</f>
-        <v>TPPUMBTELC-N</v>
+        <v>TPPRCARHGNF-N</v>
       </c>
       <c r="E11">
         <v>2055</v>
@@ -22428,26 +22474,25 @@
       </c>
       <c r="I11">
         <f>I10</f>
-        <v>-2</v>
+        <v>-10</v>
       </c>
       <c r="J11" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:11">
       <c r="B12" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UC_Growth_TFLCVOGSH-N</v>
-      </c>
-      <c r="C12" s="2" t="str">
-        <f>C8</f>
-        <v>NCAP,GROWTH</v>
+        <f>"UC_Growth_"&amp;D12</f>
+        <v>UC_Growth_TPPRSUVELC-N</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E12">
-        <f t="shared" ref="E12:E20" si="2">E6</f>
+        <f>E9</f>
         <v>2024</v>
       </c>
       <c r="F12" s="2" t="s">
@@ -22467,23 +22512,21 @@
       <c r="J12" s="2">
         <v>5</v>
       </c>
-      <c r="N12" s="2"/>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:11">
       <c r="B13" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UC_Growth_TFLCVOGSH-N</v>
+        <f t="shared" ref="B13:B14" si="2">"UC_Growth_"&amp;D13</f>
+        <v>UC_Growth_TPPRSUVELC-N</v>
       </c>
       <c r="C13" s="2" t="str">
-        <f t="shared" ref="C13:C17" si="3">C12</f>
+        <f>C12</f>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D13" s="2" t="str">
         <f>D12</f>
-        <v>TFLCVOGSH-N</v>
+        <v>TPPRSUVELC-N</v>
       </c>
       <c r="E13">
-        <f t="shared" si="2"/>
         <v>2054</v>
       </c>
       <c r="F13" s="2" t="s">
@@ -22503,23 +22546,21 @@
       <c r="J13" s="2">
         <v>5</v>
       </c>
-      <c r="N13" s="2"/>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:11">
       <c r="B14" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UC_Growth_TFLCVOGSH-N</v>
+        <f t="shared" si="2"/>
+        <v>UC_Growth_TPPRSUVELC-N</v>
       </c>
       <c r="C14" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f>C13</f>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D14" s="2" t="str">
         <f>D13</f>
-        <v>TFLCVOGSH-N</v>
+        <v>TPPRSUVELC-N</v>
       </c>
       <c r="E14">
-        <f t="shared" si="2"/>
         <v>2055</v>
       </c>
       <c r="F14" s="2" t="s">
@@ -22538,22 +22579,20 @@
       <c r="J14" s="2">
         <v>5</v>
       </c>
-      <c r="N14" s="2"/>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:11">
       <c r="B15" s="2" t="str">
-        <f t="shared" ref="B15:B17" si="4">"UC_Growth_"&amp;D15</f>
-        <v>UC_Growth_TFLCVELC-N</v>
-      </c>
-      <c r="C15" s="2" t="str">
-        <f>C11</f>
-        <v>NCAP,GROWTH</v>
+        <f>"UC_Growth_"&amp;D15</f>
+        <v>UC_Growth_TPPRSUVHGNF-N</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="E15">
-        <f t="shared" si="2"/>
+        <f>E12</f>
         <v>2024</v>
       </c>
       <c r="F15" s="2" t="s">
@@ -22573,23 +22612,21 @@
       <c r="J15" s="2">
         <v>5</v>
       </c>
-      <c r="N15" s="2"/>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:11">
       <c r="B16" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>UC_Growth_TFLCVELC-N</v>
+        <f t="shared" ref="B16:B17" si="3">"UC_Growth_"&amp;D16</f>
+        <v>UC_Growth_TPPRSUVHGNF-N</v>
       </c>
       <c r="C16" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f>C15</f>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D16" s="2" t="str">
         <f>D15</f>
-        <v>TFLCVELC-N</v>
+        <v>TPPRSUVHGNF-N</v>
       </c>
       <c r="E16">
-        <f t="shared" si="2"/>
         <v>2054</v>
       </c>
       <c r="F16" s="2" t="s">
@@ -22609,23 +22646,21 @@
       <c r="J16" s="2">
         <v>5</v>
       </c>
-      <c r="N16" s="2"/>
     </row>
     <row r="17" spans="2:14">
       <c r="B17" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>UC_Growth_TFLCVELC-N</v>
+        <f t="shared" si="3"/>
+        <v>UC_Growth_TPPRSUVHGNF-N</v>
       </c>
       <c r="C17" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f>C16</f>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D17" s="2" t="str">
         <f>D16</f>
-        <v>TFLCVELC-N</v>
+        <v>TPPRSUVHGNF-N</v>
       </c>
       <c r="E17">
-        <f t="shared" si="2"/>
         <v>2055</v>
       </c>
       <c r="F17" s="2" t="s">
@@ -22644,22 +22679,20 @@
       <c r="J17" s="2">
         <v>5</v>
       </c>
-      <c r="N17" s="2"/>
     </row>
     <row r="18" spans="2:14">
       <c r="B18" s="2" t="str">
-        <f t="shared" ref="B18:B20" si="5">"UC_Growth_"&amp;D18</f>
-        <v>UC_Growth_TFHCV1ELC-N</v>
-      </c>
-      <c r="C18" s="2" t="str">
-        <f>C14</f>
-        <v>NCAP,GROWTH</v>
+        <f>"UC_Growth_"&amp;D18</f>
+        <v>UC_Growth_TPPUMBTELC-N</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E18">
-        <f t="shared" si="2"/>
+        <f>$G$1</f>
         <v>2024</v>
       </c>
       <c r="F18" s="2" t="s">
@@ -22673,28 +22706,26 @@
         <v>1</v>
       </c>
       <c r="I18">
-        <v>-5</v>
+        <v>-2</v>
       </c>
       <c r="J18" s="2">
         <v>5</v>
       </c>
-      <c r="N18" s="2"/>
     </row>
     <row r="19" spans="2:14">
       <c r="B19" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>UC_Growth_TFHCV1ELC-N</v>
+        <f t="shared" ref="B19:B20" si="4">"UC_Growth_"&amp;D19</f>
+        <v>UC_Growth_TPPUMBTELC-N</v>
       </c>
       <c r="C19" s="2" t="str">
-        <f t="shared" ref="C19:C20" si="6">C18</f>
+        <f>C18</f>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D19" s="2" t="str">
         <f>D18</f>
-        <v>TFHCV1ELC-N</v>
+        <v>TPPUMBTELC-N</v>
       </c>
       <c r="E19">
-        <f t="shared" si="2"/>
         <v>2054</v>
       </c>
       <c r="F19" s="2" t="s">
@@ -22709,7 +22740,7 @@
       </c>
       <c r="I19">
         <f>I18</f>
-        <v>-5</v>
+        <v>-2</v>
       </c>
       <c r="J19" s="2">
         <v>5</v>
@@ -22717,19 +22748,18 @@
     </row>
     <row r="20" spans="2:14">
       <c r="B20" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>UC_Growth_TFHCV1ELC-N</v>
+        <f t="shared" si="4"/>
+        <v>UC_Growth_TPPUMBTELC-N</v>
       </c>
       <c r="C20" s="2" t="str">
-        <f t="shared" si="6"/>
+        <f>C19</f>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D20" s="2" t="str">
         <f>D19</f>
-        <v>TFHCV1ELC-N</v>
+        <v>TPPUMBTELC-N</v>
       </c>
       <c r="E20">
-        <f t="shared" si="2"/>
         <v>2055</v>
       </c>
       <c r="F20" s="2" t="s">
@@ -22743,9 +22773,1663 @@
       </c>
       <c r="I20">
         <f>I19</f>
+        <v>-2</v>
+      </c>
+      <c r="J20" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14">
+      <c r="B21" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>UC_Growth_TFLCVOGSH-N</v>
+      </c>
+      <c r="C21" s="2" t="str">
+        <f>C8</f>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21">
+        <f>E6</f>
+        <v>2024</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21">
+        <f>1+$E$1</f>
+        <v>1.2</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <f>-$E$2</f>
+        <v>-10</v>
+      </c>
+      <c r="J21" s="2">
+        <v>5</v>
+      </c>
+      <c r="N21" s="2"/>
+    </row>
+    <row r="22" spans="2:14">
+      <c r="B22" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>UC_Growth_TFLCVOGSH-N</v>
+      </c>
+      <c r="C22" s="2" t="str">
+        <f t="shared" ref="C22:C26" si="5">C21</f>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D22" s="2" t="str">
+        <f>D21</f>
+        <v>TFLCVOGSH-N</v>
+      </c>
+      <c r="E22">
+        <f>E7</f>
+        <v>2054</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22">
+        <f>1+$E$1</f>
+        <v>1.2</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <f>I21</f>
+        <v>-10</v>
+      </c>
+      <c r="J22" s="2">
+        <v>5</v>
+      </c>
+      <c r="N22" s="2"/>
+    </row>
+    <row r="23" spans="2:14">
+      <c r="B23" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>UC_Growth_TFLCVOGSH-N</v>
+      </c>
+      <c r="C23" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D23" s="2" t="str">
+        <f>D22</f>
+        <v>TFLCVOGSH-N</v>
+      </c>
+      <c r="E23">
+        <f>E8</f>
+        <v>2055</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G23">
+        <v>100</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <f>I22</f>
+        <v>-10</v>
+      </c>
+      <c r="J23" s="2">
+        <v>5</v>
+      </c>
+      <c r="N23" s="2"/>
+    </row>
+    <row r="24" spans="2:14">
+      <c r="B24" s="2" t="str">
+        <f t="shared" ref="B24:B26" si="6">"UC_Growth_"&amp;D24</f>
+        <v>UC_Growth_TFLCVELC-N</v>
+      </c>
+      <c r="C24" s="2" t="str">
+        <f>C20</f>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24">
+        <f t="shared" ref="E24:E68" si="7">E18</f>
+        <v>2024</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24">
+        <f>1+$E$1</f>
+        <v>1.2</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <f>-$E$2</f>
+        <v>-10</v>
+      </c>
+      <c r="J24" s="2">
+        <v>5</v>
+      </c>
+      <c r="N24" s="2"/>
+    </row>
+    <row r="25" spans="2:14">
+      <c r="B25" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>UC_Growth_TFLCVELC-N</v>
+      </c>
+      <c r="C25" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D25" s="2" t="str">
+        <f>D24</f>
+        <v>TFLCVELC-N</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="7"/>
+        <v>2054</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G25">
+        <f>1+$E$1</f>
+        <v>1.2</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <f>I24</f>
+        <v>-10</v>
+      </c>
+      <c r="J25" s="2">
+        <v>5</v>
+      </c>
+      <c r="N25" s="2"/>
+    </row>
+    <row r="26" spans="2:14">
+      <c r="B26" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>UC_Growth_TFLCVELC-N</v>
+      </c>
+      <c r="C26" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D26" s="2" t="str">
+        <f>D25</f>
+        <v>TFLCVELC-N</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="7"/>
+        <v>2055</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G26">
+        <v>100</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <f>I25</f>
+        <v>-10</v>
+      </c>
+      <c r="J26" s="2">
+        <v>5</v>
+      </c>
+      <c r="N26" s="2"/>
+    </row>
+    <row r="27" spans="2:14">
+      <c r="B27" s="2" t="str">
+        <f t="shared" ref="B27:B29" si="8">"UC_Growth_"&amp;D27</f>
+        <v>UC_Growth_TFHCV1ELC-N</v>
+      </c>
+      <c r="C27" s="2" t="str">
+        <f>C23</f>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="7"/>
+        <v>2024</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27">
+        <f>1+$E$1</f>
+        <v>1.2</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
         <v>-5</v>
       </c>
-      <c r="J20" s="2">
+      <c r="J27" s="2">
+        <v>5</v>
+      </c>
+      <c r="N27" s="2"/>
+    </row>
+    <row r="28" spans="2:14">
+      <c r="B28" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v>UC_Growth_TFHCV1ELC-N</v>
+      </c>
+      <c r="C28" s="2" t="str">
+        <f t="shared" ref="C28:C68" si="9">C27</f>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D28" s="2" t="str">
+        <f>D27</f>
+        <v>TFHCV1ELC-N</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="7"/>
+        <v>2054</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G28">
+        <f>1+$E$1</f>
+        <v>1.2</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <f>I27</f>
+        <v>-5</v>
+      </c>
+      <c r="J28" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14">
+      <c r="B29" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v>UC_Growth_TFHCV1ELC-N</v>
+      </c>
+      <c r="C29" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D29" s="2" t="str">
+        <f>D28</f>
+        <v>TFHCV1ELC-N</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="7"/>
+        <v>2055</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G29">
+        <v>100</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <f>I28</f>
+        <v>-5</v>
+      </c>
+      <c r="J29" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14">
+      <c r="B30" s="2" t="str">
+        <f t="shared" ref="B30:B53" si="10">"UC_Growth_"&amp;D30</f>
+        <v>UC_Growth_TFHCV2ELC-N</v>
+      </c>
+      <c r="C30" s="2" t="str">
+        <f>C26</f>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="7"/>
+        <v>2024</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G30">
+        <f>1+$E$1</f>
+        <v>1.2</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <v>2</v>
+      </c>
+      <c r="J30" s="2">
+        <v>5</v>
+      </c>
+      <c r="N30" s="2"/>
+    </row>
+    <row r="31" spans="2:14">
+      <c r="B31" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>UC_Growth_TFHCV2ELC-N</v>
+      </c>
+      <c r="C31" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D31" s="2" t="str">
+        <f>D30</f>
+        <v>TFHCV2ELC-N</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="7"/>
+        <v>2054</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G31">
+        <f>1+$E$1</f>
+        <v>1.2</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <f>I30</f>
+        <v>2</v>
+      </c>
+      <c r="J31" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14">
+      <c r="B32" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>UC_Growth_TFHCV2ELC-N</v>
+      </c>
+      <c r="C32" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D32" s="2" t="str">
+        <f>D31</f>
+        <v>TFHCV2ELC-N</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="7"/>
+        <v>2055</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G32">
+        <v>100</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <f>I31</f>
+        <v>2</v>
+      </c>
+      <c r="J32" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14">
+      <c r="B33" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>UC_Growth_TFHCV3ELC-N</v>
+      </c>
+      <c r="C33" s="2" t="str">
+        <f>C29</f>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="7"/>
+        <v>2024</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G33">
+        <f>1+$E$1</f>
+        <v>1.2</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="I33">
+        <v>2</v>
+      </c>
+      <c r="J33" s="2">
+        <v>5</v>
+      </c>
+      <c r="N33" s="2"/>
+    </row>
+    <row r="34" spans="2:14">
+      <c r="B34" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>UC_Growth_TFHCV3ELC-N</v>
+      </c>
+      <c r="C34" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D34" s="2" t="str">
+        <f>D33</f>
+        <v>TFHCV3ELC-N</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="7"/>
+        <v>2054</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G34">
+        <f>1+$E$1</f>
+        <v>1.2</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="I34">
+        <f>I33</f>
+        <v>2</v>
+      </c>
+      <c r="J34" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14">
+      <c r="B35" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>UC_Growth_TFHCV3ELC-N</v>
+      </c>
+      <c r="C35" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D35" s="2" t="str">
+        <f>D34</f>
+        <v>TFHCV3ELC-N</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="7"/>
+        <v>2055</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G35">
+        <v>100</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+      <c r="I35">
+        <f>I34</f>
+        <v>2</v>
+      </c>
+      <c r="J35" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14">
+      <c r="B36" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>UC_Growth_TFHCV4ELC-N</v>
+      </c>
+      <c r="C36" s="2" t="str">
+        <f>C32</f>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="7"/>
+        <v>2024</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G36">
+        <f>1+$E$1</f>
+        <v>1.2</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="I36">
+        <v>2</v>
+      </c>
+      <c r="J36" s="2">
+        <v>5</v>
+      </c>
+      <c r="N36" s="2"/>
+    </row>
+    <row r="37" spans="2:14">
+      <c r="B37" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>UC_Growth_TFHCV4ELC-N</v>
+      </c>
+      <c r="C37" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D37" s="2" t="str">
+        <f>D36</f>
+        <v>TFHCV4ELC-N</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="7"/>
+        <v>2054</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G37">
+        <f>1+$E$1</f>
+        <v>1.2</v>
+      </c>
+      <c r="H37">
+        <v>1</v>
+      </c>
+      <c r="I37">
+        <f>I36</f>
+        <v>2</v>
+      </c>
+      <c r="J37" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14">
+      <c r="B38" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>UC_Growth_TFHCV4ELC-N</v>
+      </c>
+      <c r="C38" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D38" s="2" t="str">
+        <f>D37</f>
+        <v>TFHCV4ELC-N</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="7"/>
+        <v>2055</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G38">
+        <v>100</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="I38">
+        <f>I37</f>
+        <v>2</v>
+      </c>
+      <c r="J38" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="2:14">
+      <c r="B39" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>UC_Growth_TFHCV5ELC-N</v>
+      </c>
+      <c r="C39" s="2" t="str">
+        <f>C35</f>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="7"/>
+        <v>2024</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G39">
+        <f>1+$E$1</f>
+        <v>1.2</v>
+      </c>
+      <c r="H39">
+        <v>1</v>
+      </c>
+      <c r="I39">
+        <v>2</v>
+      </c>
+      <c r="J39" s="2">
+        <v>5</v>
+      </c>
+      <c r="N39" s="2"/>
+    </row>
+    <row r="40" spans="2:14">
+      <c r="B40" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>UC_Growth_TFHCV5ELC-N</v>
+      </c>
+      <c r="C40" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D40" s="2" t="str">
+        <f>D39</f>
+        <v>TFHCV5ELC-N</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="7"/>
+        <v>2054</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G40">
+        <f>1+$E$1</f>
+        <v>1.2</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+      <c r="I40">
+        <f>I39</f>
+        <v>2</v>
+      </c>
+      <c r="J40" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="2:14">
+      <c r="B41" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>UC_Growth_TFHCV5ELC-N</v>
+      </c>
+      <c r="C41" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D41" s="2" t="str">
+        <f>D40</f>
+        <v>TFHCV5ELC-N</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="7"/>
+        <v>2055</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G41">
+        <v>100</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+      <c r="I41">
+        <f>I40</f>
+        <v>2</v>
+      </c>
+      <c r="J41" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="2:14">
+      <c r="B42" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>UC_Growth_TFHCV6ELC-N</v>
+      </c>
+      <c r="C42" s="2" t="str">
+        <f>C38</f>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="7"/>
+        <v>2024</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G42">
+        <f>1+$E$1</f>
+        <v>1.2</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="I42">
+        <v>-2</v>
+      </c>
+      <c r="J42" s="2">
+        <v>5</v>
+      </c>
+      <c r="N42" s="2"/>
+    </row>
+    <row r="43" spans="2:14">
+      <c r="B43" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>UC_Growth_TFHCV6ELC-N</v>
+      </c>
+      <c r="C43" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D43" s="2" t="str">
+        <f>D42</f>
+        <v>TFHCV6ELC-N</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="7"/>
+        <v>2054</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G43">
+        <f>1+$E$1</f>
+        <v>1.2</v>
+      </c>
+      <c r="H43">
+        <v>1</v>
+      </c>
+      <c r="I43">
+        <f>I42</f>
+        <v>-2</v>
+      </c>
+      <c r="J43" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="2:14">
+      <c r="B44" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>UC_Growth_TFHCV6ELC-N</v>
+      </c>
+      <c r="C44" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D44" s="2" t="str">
+        <f>D43</f>
+        <v>TFHCV6ELC-N</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="7"/>
+        <v>2055</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G44">
+        <v>100</v>
+      </c>
+      <c r="H44">
+        <v>1</v>
+      </c>
+      <c r="I44">
+        <f>I43</f>
+        <v>-2</v>
+      </c>
+      <c r="J44" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="2:14">
+      <c r="B45" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>UC_Growth_TFHCV7ELC-N</v>
+      </c>
+      <c r="C45" s="2" t="str">
+        <f>C41</f>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="7"/>
+        <v>2024</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G45">
+        <f>1+$E$1</f>
+        <v>1.2</v>
+      </c>
+      <c r="H45">
+        <v>1</v>
+      </c>
+      <c r="I45">
+        <v>-2</v>
+      </c>
+      <c r="J45" s="2">
+        <v>5</v>
+      </c>
+      <c r="N45" s="2"/>
+    </row>
+    <row r="46" spans="2:14">
+      <c r="B46" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>UC_Growth_TFHCV7ELC-N</v>
+      </c>
+      <c r="C46" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D46" s="2" t="str">
+        <f>D45</f>
+        <v>TFHCV7ELC-N</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="7"/>
+        <v>2054</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G46">
+        <f>1+$E$1</f>
+        <v>1.2</v>
+      </c>
+      <c r="H46">
+        <v>1</v>
+      </c>
+      <c r="I46">
+        <f>I45</f>
+        <v>-2</v>
+      </c>
+      <c r="J46" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="2:14">
+      <c r="B47" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>UC_Growth_TFHCV7ELC-N</v>
+      </c>
+      <c r="C47" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D47" s="2" t="str">
+        <f>D46</f>
+        <v>TFHCV7ELC-N</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="7"/>
+        <v>2055</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G47">
+        <v>100</v>
+      </c>
+      <c r="H47">
+        <v>1</v>
+      </c>
+      <c r="I47">
+        <f>I46</f>
+        <v>-2</v>
+      </c>
+      <c r="J47" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="2:14">
+      <c r="B48" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>UC_Growth_TFHCV1ELC-N</v>
+      </c>
+      <c r="C48" s="2" t="str">
+        <f>C44</f>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="7"/>
+        <v>2024</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G48">
+        <f>1+$E$1</f>
+        <v>1.2</v>
+      </c>
+      <c r="H48">
+        <v>1</v>
+      </c>
+      <c r="I48">
+        <v>-5</v>
+      </c>
+      <c r="J48" s="2">
+        <v>5</v>
+      </c>
+      <c r="N48" s="2"/>
+    </row>
+    <row r="49" spans="2:14">
+      <c r="B49" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>UC_Growth_TFHCV1ELC-N</v>
+      </c>
+      <c r="C49" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D49" s="2" t="str">
+        <f>D48</f>
+        <v>TFHCV1ELC-N</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="7"/>
+        <v>2054</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G49">
+        <f>1+$E$1</f>
+        <v>1.2</v>
+      </c>
+      <c r="H49">
+        <v>1</v>
+      </c>
+      <c r="I49">
+        <f>I48</f>
+        <v>-5</v>
+      </c>
+      <c r="J49" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="2:14">
+      <c r="B50" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>UC_Growth_TFHCV1ELC-N</v>
+      </c>
+      <c r="C50" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D50" s="2" t="str">
+        <f>D49</f>
+        <v>TFHCV1ELC-N</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="7"/>
+        <v>2055</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G50">
+        <v>100</v>
+      </c>
+      <c r="H50">
+        <v>1</v>
+      </c>
+      <c r="I50">
+        <f>I49</f>
+        <v>-5</v>
+      </c>
+      <c r="J50" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="2:14">
+      <c r="B51" s="2" t="str">
+        <f t="shared" ref="B51:B68" si="11">"UC_Growth_"&amp;D51</f>
+        <v>UC_Growth_TFHCV2HGN-N</v>
+      </c>
+      <c r="C51" s="2" t="str">
+        <f>C47</f>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D51" t="s">
+        <v>75</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="7"/>
+        <v>2024</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G51">
+        <f>1+$E$1</f>
+        <v>1.2</v>
+      </c>
+      <c r="H51">
+        <v>1</v>
+      </c>
+      <c r="I51">
+        <v>2</v>
+      </c>
+      <c r="J51" s="2">
+        <v>5</v>
+      </c>
+      <c r="N51" s="2"/>
+    </row>
+    <row r="52" spans="2:14">
+      <c r="B52" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>UC_Growth_TFHCV2HGN-N</v>
+      </c>
+      <c r="C52" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D52" s="2" t="str">
+        <f>D51</f>
+        <v>TFHCV2HGN-N</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="7"/>
+        <v>2054</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G52">
+        <f>1+$E$1</f>
+        <v>1.2</v>
+      </c>
+      <c r="H52">
+        <v>1</v>
+      </c>
+      <c r="I52">
+        <f>I51</f>
+        <v>2</v>
+      </c>
+      <c r="J52" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="2:14">
+      <c r="B53" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>UC_Growth_TFHCV2HGN-N</v>
+      </c>
+      <c r="C53" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D53" s="2" t="str">
+        <f>D52</f>
+        <v>TFHCV2HGN-N</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="7"/>
+        <v>2055</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G53">
+        <v>100</v>
+      </c>
+      <c r="H53">
+        <v>1</v>
+      </c>
+      <c r="I53">
+        <f>I52</f>
+        <v>2</v>
+      </c>
+      <c r="J53" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="2:14">
+      <c r="B54" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>UC_Growth_TFHCV3HGN-N</v>
+      </c>
+      <c r="C54" s="2" t="str">
+        <f>C50</f>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D54" t="s">
+        <v>76</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="7"/>
+        <v>2024</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G54">
+        <f>1+$E$1</f>
+        <v>1.2</v>
+      </c>
+      <c r="H54">
+        <v>1</v>
+      </c>
+      <c r="I54">
+        <v>2</v>
+      </c>
+      <c r="J54" s="2">
+        <v>5</v>
+      </c>
+      <c r="N54" s="2"/>
+    </row>
+    <row r="55" spans="2:14">
+      <c r="B55" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>UC_Growth_TFHCV3HGN-N</v>
+      </c>
+      <c r="C55" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D55" s="2" t="str">
+        <f>D54</f>
+        <v>TFHCV3HGN-N</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="7"/>
+        <v>2054</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G55">
+        <f>1+$E$1</f>
+        <v>1.2</v>
+      </c>
+      <c r="H55">
+        <v>1</v>
+      </c>
+      <c r="I55">
+        <f>I54</f>
+        <v>2</v>
+      </c>
+      <c r="J55" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="2:14">
+      <c r="B56" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>UC_Growth_TFHCV3HGN-N</v>
+      </c>
+      <c r="C56" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D56" s="2" t="str">
+        <f>D55</f>
+        <v>TFHCV3HGN-N</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="7"/>
+        <v>2055</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G56">
+        <v>100</v>
+      </c>
+      <c r="H56">
+        <v>1</v>
+      </c>
+      <c r="I56">
+        <f>I55</f>
+        <v>2</v>
+      </c>
+      <c r="J56" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="2:14">
+      <c r="B57" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>UC_Growth_TFHCV4HGN-N</v>
+      </c>
+      <c r="C57" s="2" t="str">
+        <f>C53</f>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D57" t="s">
+        <v>77</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="7"/>
+        <v>2024</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G57">
+        <f>1+$E$1</f>
+        <v>1.2</v>
+      </c>
+      <c r="H57">
+        <v>1</v>
+      </c>
+      <c r="I57">
+        <v>2</v>
+      </c>
+      <c r="J57" s="2">
+        <v>5</v>
+      </c>
+      <c r="N57" s="2"/>
+    </row>
+    <row r="58" spans="2:14">
+      <c r="B58" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>UC_Growth_TFHCV4HGN-N</v>
+      </c>
+      <c r="C58" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D58" s="2" t="str">
+        <f>D57</f>
+        <v>TFHCV4HGN-N</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="7"/>
+        <v>2054</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G58">
+        <f>1+$E$1</f>
+        <v>1.2</v>
+      </c>
+      <c r="H58">
+        <v>1</v>
+      </c>
+      <c r="I58">
+        <f>I57</f>
+        <v>2</v>
+      </c>
+      <c r="J58" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="2:14">
+      <c r="B59" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>UC_Growth_TFHCV4HGN-N</v>
+      </c>
+      <c r="C59" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D59" s="2" t="str">
+        <f>D58</f>
+        <v>TFHCV4HGN-N</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="7"/>
+        <v>2055</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G59">
+        <v>100</v>
+      </c>
+      <c r="H59">
+        <v>1</v>
+      </c>
+      <c r="I59">
+        <f>I58</f>
+        <v>2</v>
+      </c>
+      <c r="J59" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="2:14">
+      <c r="B60" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>UC_Growth_TFHCV5HGN-N</v>
+      </c>
+      <c r="C60" s="2" t="str">
+        <f>C56</f>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D60" t="s">
+        <v>78</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="7"/>
+        <v>2024</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G60">
+        <f>1+$E$1</f>
+        <v>1.2</v>
+      </c>
+      <c r="H60">
+        <v>1</v>
+      </c>
+      <c r="I60">
+        <v>2</v>
+      </c>
+      <c r="J60" s="2">
+        <v>5</v>
+      </c>
+      <c r="N60" s="2"/>
+    </row>
+    <row r="61" spans="2:14">
+      <c r="B61" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>UC_Growth_TFHCV5HGN-N</v>
+      </c>
+      <c r="C61" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D61" s="2" t="str">
+        <f>D60</f>
+        <v>TFHCV5HGN-N</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="7"/>
+        <v>2054</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G61">
+        <f>1+$E$1</f>
+        <v>1.2</v>
+      </c>
+      <c r="H61">
+        <v>1</v>
+      </c>
+      <c r="I61">
+        <f>I60</f>
+        <v>2</v>
+      </c>
+      <c r="J61" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="2:14">
+      <c r="B62" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>UC_Growth_TFHCV5HGN-N</v>
+      </c>
+      <c r="C62" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D62" s="2" t="str">
+        <f>D61</f>
+        <v>TFHCV5HGN-N</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="7"/>
+        <v>2055</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G62">
+        <v>100</v>
+      </c>
+      <c r="H62">
+        <v>1</v>
+      </c>
+      <c r="I62">
+        <f>I61</f>
+        <v>2</v>
+      </c>
+      <c r="J62" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="2:14">
+      <c r="B63" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>UC_Growth_TFHCV6HGN-N</v>
+      </c>
+      <c r="C63" s="2" t="str">
+        <f>C59</f>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D63" t="s">
+        <v>79</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="7"/>
+        <v>2024</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G63">
+        <f>1+$E$1</f>
+        <v>1.2</v>
+      </c>
+      <c r="H63">
+        <v>1</v>
+      </c>
+      <c r="I63">
+        <v>-2</v>
+      </c>
+      <c r="J63" s="2">
+        <v>5</v>
+      </c>
+      <c r="N63" s="2"/>
+    </row>
+    <row r="64" spans="2:14">
+      <c r="B64" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>UC_Growth_TFHCV6HGN-N</v>
+      </c>
+      <c r="C64" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D64" s="2" t="str">
+        <f>D63</f>
+        <v>TFHCV6HGN-N</v>
+      </c>
+      <c r="E64">
+        <f t="shared" si="7"/>
+        <v>2054</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G64">
+        <f>1+$E$1</f>
+        <v>1.2</v>
+      </c>
+      <c r="H64">
+        <v>1</v>
+      </c>
+      <c r="I64">
+        <f>I63</f>
+        <v>-2</v>
+      </c>
+      <c r="J64" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="2:14">
+      <c r="B65" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>UC_Growth_TFHCV6HGN-N</v>
+      </c>
+      <c r="C65" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D65" s="2" t="str">
+        <f>D64</f>
+        <v>TFHCV6HGN-N</v>
+      </c>
+      <c r="E65">
+        <f t="shared" si="7"/>
+        <v>2055</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G65">
+        <v>100</v>
+      </c>
+      <c r="H65">
+        <v>1</v>
+      </c>
+      <c r="I65">
+        <f>I64</f>
+        <v>-2</v>
+      </c>
+      <c r="J65" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="2:14">
+      <c r="B66" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>UC_Growth_TFHCV7HGN-N</v>
+      </c>
+      <c r="C66" s="2" t="str">
+        <f>C62</f>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D66" t="s">
+        <v>80</v>
+      </c>
+      <c r="E66">
+        <f t="shared" si="7"/>
+        <v>2024</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G66">
+        <f>1+$E$1</f>
+        <v>1.2</v>
+      </c>
+      <c r="H66">
+        <v>1</v>
+      </c>
+      <c r="I66">
+        <v>-2</v>
+      </c>
+      <c r="J66" s="2">
+        <v>5</v>
+      </c>
+      <c r="N66" s="2"/>
+    </row>
+    <row r="67" spans="2:14">
+      <c r="B67" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>UC_Growth_TFHCV7HGN-N</v>
+      </c>
+      <c r="C67" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D67" s="2" t="str">
+        <f>D66</f>
+        <v>TFHCV7HGN-N</v>
+      </c>
+      <c r="E67">
+        <f t="shared" si="7"/>
+        <v>2054</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G67">
+        <f>1+$E$1</f>
+        <v>1.2</v>
+      </c>
+      <c r="H67">
+        <v>1</v>
+      </c>
+      <c r="I67">
+        <f>I66</f>
+        <v>-2</v>
+      </c>
+      <c r="J67" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="2:14">
+      <c r="B68" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>UC_Growth_TFHCV7HGN-N</v>
+      </c>
+      <c r="C68" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D68" s="2" t="str">
+        <f>D67</f>
+        <v>TFHCV7HGN-N</v>
+      </c>
+      <c r="E68">
+        <f t="shared" si="7"/>
+        <v>2055</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G68">
+        <v>100</v>
+      </c>
+      <c r="H68">
+        <v>1</v>
+      </c>
+      <c r="I68">
+        <f>I67</f>
+        <v>-2</v>
+      </c>
+      <c r="J68" s="2">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
UC ELC (transport growth) error fixed
</commit_message>
<xml_diff>
--- a/suppxls/Scen_UC_ELC.xlsx
+++ b/suppxls/Scen_UC_ELC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\suppxls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0901D2C-3FC3-4C47-9E5A-2EE9D305F3B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF4CC60-21C4-4236-BD34-06B9CA29ACD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4065" yWindow="-19140" windowWidth="26610" windowHeight="13740" firstSheet="5" activeTab="8" xr2:uid="{22D7DAD2-FC1B-44BE-801D-D5E60FB61EEE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="8" xr2:uid="{22D7DAD2-FC1B-44BE-801D-D5E60FB61EEE}"/>
   </bookViews>
   <sheets>
     <sheet name="BuildRateConstraints" sheetId="1" r:id="rId1"/>
@@ -22194,7 +22194,7 @@
   <dimension ref="A1:N68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71:B76"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -23096,7 +23096,7 @@
     </row>
     <row r="30" spans="2:14">
       <c r="B30" s="2" t="str">
-        <f t="shared" ref="B30:B53" si="10">"UC_Growth_"&amp;D30</f>
+        <f t="shared" ref="B30:B50" si="10">"UC_Growth_"&amp;D30</f>
         <v>UC_Growth_TFHCV2ELC-N</v>
       </c>
       <c r="C30" s="2" t="str">
@@ -23121,7 +23121,7 @@
         <v>1</v>
       </c>
       <c r="I30">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="J30" s="2">
         <v>5</v>
@@ -23157,7 +23157,7 @@
       </c>
       <c r="I31">
         <f>I30</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="J31" s="2">
         <v>5</v>
@@ -23191,7 +23191,7 @@
       </c>
       <c r="I32">
         <f>I31</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="J32" s="2">
         <v>5</v>
@@ -23224,7 +23224,7 @@
         <v>1</v>
       </c>
       <c r="I33">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="J33" s="2">
         <v>5</v>
@@ -23260,7 +23260,7 @@
       </c>
       <c r="I34">
         <f>I33</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="J34" s="2">
         <v>5</v>
@@ -23294,7 +23294,7 @@
       </c>
       <c r="I35">
         <f>I34</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="J35" s="2">
         <v>5</v>
@@ -23327,7 +23327,7 @@
         <v>1</v>
       </c>
       <c r="I36">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="J36" s="2">
         <v>5</v>
@@ -23363,7 +23363,7 @@
       </c>
       <c r="I37">
         <f>I36</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="J37" s="2">
         <v>5</v>
@@ -23397,7 +23397,7 @@
       </c>
       <c r="I38">
         <f>I37</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="J38" s="2">
         <v>5</v>
@@ -23430,7 +23430,7 @@
         <v>1</v>
       </c>
       <c r="I39">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="J39" s="2">
         <v>5</v>
@@ -23466,7 +23466,7 @@
       </c>
       <c r="I40">
         <f>I39</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="J40" s="2">
         <v>5</v>
@@ -23500,7 +23500,7 @@
       </c>
       <c r="I41">
         <f>I40</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="J41" s="2">
         <v>5</v>
@@ -23842,7 +23842,7 @@
         <v>1</v>
       </c>
       <c r="I51">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="J51" s="2">
         <v>5</v>
@@ -23878,7 +23878,7 @@
       </c>
       <c r="I52">
         <f>I51</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="J52" s="2">
         <v>5</v>
@@ -23912,7 +23912,7 @@
       </c>
       <c r="I53">
         <f>I52</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="J53" s="2">
         <v>5</v>
@@ -23945,7 +23945,7 @@
         <v>1</v>
       </c>
       <c r="I54">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="J54" s="2">
         <v>5</v>
@@ -23981,7 +23981,7 @@
       </c>
       <c r="I55">
         <f>I54</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="J55" s="2">
         <v>5</v>
@@ -24015,7 +24015,7 @@
       </c>
       <c r="I56">
         <f>I55</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="J56" s="2">
         <v>5</v>
@@ -24048,7 +24048,7 @@
         <v>1</v>
       </c>
       <c r="I57">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="J57" s="2">
         <v>5</v>
@@ -24084,7 +24084,7 @@
       </c>
       <c r="I58">
         <f>I57</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="J58" s="2">
         <v>5</v>
@@ -24118,7 +24118,7 @@
       </c>
       <c r="I59">
         <f>I58</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="J59" s="2">
         <v>5</v>
@@ -24151,7 +24151,7 @@
         <v>1</v>
       </c>
       <c r="I60">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="J60" s="2">
         <v>5</v>
@@ -24187,7 +24187,7 @@
       </c>
       <c r="I61">
         <f>I60</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="J61" s="2">
         <v>5</v>
@@ -24221,7 +24221,7 @@
       </c>
       <c r="I62">
         <f>I61</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="J62" s="2">
         <v>5</v>

</xml_diff>

<commit_message>
UC Growth on INDHGN error fixed
</commit_message>
<xml_diff>
--- a/suppxls/Scen_UC_ELC.xlsx
+++ b/suppxls/Scen_UC_ELC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\suppxls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF4CC60-21C4-4236-BD34-06B9CA29ACD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C0069E-07BD-4096-9C8F-3240EB53F774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="8" xr2:uid="{22D7DAD2-FC1B-44BE-801D-D5E60FB61EEE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="7" xr2:uid="{22D7DAD2-FC1B-44BE-801D-D5E60FB61EEE}"/>
   </bookViews>
   <sheets>
     <sheet name="BuildRateConstraints" sheetId="1" r:id="rId1"/>
@@ -21487,8 +21487,8 @@
   </sheetPr>
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -22003,8 +22003,8 @@
         <v>1</v>
       </c>
       <c r="I18">
-        <f>I15</f>
-        <v>0</v>
+        <f>-E3</f>
+        <v>-10</v>
       </c>
       <c r="J18" s="2">
         <v>5</v>
@@ -22036,8 +22036,8 @@
         <v>1</v>
       </c>
       <c r="I19">
-        <f>I16</f>
-        <v>0</v>
+        <f>I18</f>
+        <v>-10</v>
       </c>
       <c r="J19" s="2">
         <v>5</v>
@@ -22068,8 +22068,8 @@
         <v>1</v>
       </c>
       <c r="I20">
-        <f>I17</f>
-        <v>0</v>
+        <f>I19</f>
+        <v>-10</v>
       </c>
       <c r="J20" s="2">
         <v>5</v>
@@ -22193,7 +22193,7 @@
   </sheetPr>
   <dimension ref="A1:N68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
with growth constraints on CSP and DAC
</commit_message>
<xml_diff>
--- a/suppxls/Scen_UC_ELC.xlsx
+++ b/suppxls/Scen_UC_ELC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\suppxls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C0069E-07BD-4096-9C8F-3240EB53F774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349F5AB7-BC3E-412B-9BEA-1A749F0EA7A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="7" xr2:uid="{22D7DAD2-FC1B-44BE-801D-D5E60FB61EEE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="6" xr2:uid="{22D7DAD2-FC1B-44BE-801D-D5E60FB61EEE}"/>
   </bookViews>
   <sheets>
     <sheet name="BuildRateConstraints" sheetId="1" r:id="rId1"/>
@@ -2021,7 +2021,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="85">
   <si>
     <t>UP</t>
   </si>
@@ -2149,9 +2149,6 @@
     <t>ERSOLP*</t>
   </si>
   <si>
-    <t>UC_Growth_Solar</t>
-  </si>
-  <si>
     <t>UC_Growth_Batteries</t>
   </si>
   <si>
@@ -2264,6 +2261,21 @@
   </si>
   <si>
     <t>TFHCV7HGN-N</t>
+  </si>
+  <si>
+    <t>UC_Growth_PV</t>
+  </si>
+  <si>
+    <t>UC_Growth_CSP</t>
+  </si>
+  <si>
+    <t>UC_Growth_DAC</t>
+  </si>
+  <si>
+    <t>ERSOLT*</t>
+  </si>
+  <si>
+    <t>UDACCO2*</t>
   </si>
 </sst>
 </file>
@@ -20724,7 +20736,7 @@
         <v>32</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>4</v>
@@ -20732,7 +20744,7 @@
     </row>
     <row r="6" spans="1:13">
       <c r="B6" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>2</v>
@@ -20753,7 +20765,7 @@
     </row>
     <row r="7" spans="1:13">
       <c r="B7" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>31</v>
@@ -20771,7 +20783,7 @@
     </row>
     <row r="8" spans="1:13">
       <c r="B8" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D8" s="2" t="str">
         <f>D6</f>
@@ -20793,7 +20805,7 @@
     </row>
     <row r="9" spans="1:13">
       <c r="B9" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D9" s="2" t="str">
         <f>D7</f>
@@ -20904,7 +20916,7 @@
         <v>32</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>4</v>
@@ -21002,10 +21014,10 @@
   <sheetPr>
     <tabColor theme="8"/>
   </sheetPr>
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -21030,7 +21042,7 @@
         <v>0.1</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G1">
         <v>2026</v>
@@ -21187,7 +21199,7 @@
     </row>
     <row r="9" spans="1:14">
       <c r="B9" s="2" t="s">
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>36</v>
@@ -21220,7 +21232,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="B10" s="2" t="s">
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>36</v>
@@ -21253,7 +21265,7 @@
     </row>
     <row r="11" spans="1:14">
       <c r="B11" s="2" t="s">
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>36</v>
@@ -21286,13 +21298,13 @@
     </row>
     <row r="12" spans="1:14">
       <c r="B12" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
@@ -21317,13 +21329,13 @@
     </row>
     <row r="13" spans="1:14">
       <c r="B13" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
@@ -21380,13 +21392,13 @@
     </row>
     <row r="15" spans="1:14">
       <c r="B15" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
@@ -21441,7 +21453,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="2:10">
+    <row r="17" spans="2:14">
       <c r="B17" s="2" t="str">
         <f>B15</f>
         <v>UC_Growth_Nuclear</v>
@@ -21474,6 +21486,199 @@
       <c r="J17" s="2">
         <v>5</v>
       </c>
+    </row>
+    <row r="18" spans="2:14">
+      <c r="B18" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E18">
+        <f>E15</f>
+        <v>2026</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18">
+        <f>G15</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <f>I15</f>
+        <v>-1</v>
+      </c>
+      <c r="J18" s="2">
+        <v>5</v>
+      </c>
+      <c r="N18" s="2"/>
+    </row>
+    <row r="19" spans="2:14">
+      <c r="B19" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19">
+        <f>E16</f>
+        <v>2054</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19">
+        <f>G16</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <f t="shared" ref="I19:I23" si="3">I16</f>
+        <v>-1</v>
+      </c>
+      <c r="J19" s="2">
+        <v>5</v>
+      </c>
+      <c r="N19" s="2"/>
+    </row>
+    <row r="20" spans="2:14">
+      <c r="B20" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E20">
+        <f t="shared" ref="E20" si="4">E17</f>
+        <v>2055</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20">
+        <f t="shared" ref="G20" si="5">G17</f>
+        <v>100</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="3"/>
+        <v>-1</v>
+      </c>
+      <c r="J20" s="2">
+        <v>5</v>
+      </c>
+      <c r="N20" s="2"/>
+    </row>
+    <row r="21" spans="2:14">
+      <c r="B21" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E21">
+        <f>E18</f>
+        <v>2026</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21">
+        <v>1.2</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>-1000</v>
+      </c>
+      <c r="J21" s="2">
+        <v>5</v>
+      </c>
+      <c r="N21" s="2"/>
+    </row>
+    <row r="22" spans="2:14">
+      <c r="B22" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E22">
+        <f>E19</f>
+        <v>2054</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22">
+        <v>1.2</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>-1000</v>
+      </c>
+      <c r="J22" s="2">
+        <v>5</v>
+      </c>
+      <c r="N22" s="2"/>
+    </row>
+    <row r="23" spans="2:14">
+      <c r="B23" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E23">
+        <f t="shared" ref="E23" si="6">E20</f>
+        <v>2055</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G23">
+        <f t="shared" ref="G23" si="7">G20</f>
+        <v>100</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>-1000</v>
+      </c>
+      <c r="J23" s="2">
+        <v>5</v>
+      </c>
+      <c r="N23" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -21487,7 +21692,7 @@
   </sheetPr>
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
@@ -21513,7 +21718,7 @@
         <v>0.1</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G1">
         <v>2026</v>
@@ -21524,7 +21729,7 @@
         <v>18</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -21535,7 +21740,7 @@
         <v>17</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E3">
         <v>10</v>
@@ -21566,7 +21771,7 @@
         <v>32</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I5" s="11" t="str">
         <f>"UC_RHSRT~"&amp;G1</f>
@@ -21585,10 +21790,10 @@
         <v>UC_Growth_XINDELC</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E6">
         <f>G1</f>
@@ -21618,7 +21823,7 @@
         <v>UC_Growth_XINDELC</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D7" s="2" t="str">
         <f>D6</f>
@@ -21651,7 +21856,7 @@
         <v>UC_Growth_XINDELC</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D8" s="2" t="str">
         <f>D7</f>
@@ -21683,10 +21888,10 @@
         <v>UC_Growth_XICPELC</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E9">
         <f>E6</f>
@@ -21716,7 +21921,7 @@
         <v>UC_Growth_XICPELC</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D10" s="2" t="str">
         <f>D9</f>
@@ -21750,7 +21955,7 @@
         <v>UC_Growth_XICPELC</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D11" s="2" t="str">
         <f>D10</f>
@@ -21783,10 +21988,10 @@
         <v>UC_Growth_XIMIELC</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E12">
         <f t="shared" si="2"/>
@@ -21816,7 +22021,7 @@
         <v>UC_Growth_XIMIELC</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D13" s="2" t="str">
         <f>D12</f>
@@ -21850,7 +22055,7 @@
         <v>UC_Growth_XIMIELC</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D14" s="2" t="str">
         <f>D13</f>
@@ -21883,10 +22088,10 @@
         <v>UC_Growth_XIFBELC</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E15">
         <f t="shared" si="2"/>
@@ -21916,7 +22121,7 @@
         <v>UC_Growth_XIFBELC</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D16" s="2" t="str">
         <f>D15</f>
@@ -21950,7 +22155,7 @@
         <v>UC_Growth_XIFBELC</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D17" s="2" t="str">
         <f>D16</f>
@@ -21983,10 +22188,10 @@
         <v>UC_Growth_XINDHGN</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E18">
         <f>E15</f>
@@ -22016,10 +22221,10 @@
         <v>UC_Growth_XINDHGN</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E19">
         <f>E16</f>
@@ -22049,10 +22254,10 @@
         <v>UC_Growth_XINDHGN</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E20">
         <f>E17</f>
@@ -22081,10 +22286,10 @@
         <v>UC_Growth_XTRAELC</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E21">
         <f>E15</f>
@@ -22115,7 +22320,7 @@
         <v>UC_Growth_XTRAELC</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D22" s="2" t="str">
         <f>D21</f>
@@ -22150,7 +22355,7 @@
         <v>UC_Growth_XTRAELC</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D23" s="2" t="str">
         <f>D22</f>
@@ -22219,7 +22424,7 @@
         <v>0.2</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G1">
         <v>2024</v>
@@ -22230,7 +22435,7 @@
         <v>18</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E2">
         <v>10</v>
@@ -22289,7 +22494,7 @@
         <v>36</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E6">
         <f>G1</f>
@@ -22389,7 +22594,7 @@
         <v>36</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E9">
         <f>E6</f>
@@ -22489,7 +22694,7 @@
         <v>36</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E12">
         <f>E9</f>
@@ -22589,7 +22794,7 @@
         <v>36</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E15">
         <f>E12</f>
@@ -22689,7 +22894,7 @@
         <v>36</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E18">
         <f>$G$1</f>
@@ -22789,7 +22994,7 @@
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E21">
         <f>E6</f>
@@ -22895,7 +23100,7 @@
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E24">
         <f t="shared" ref="E24:E68" si="7">E18</f>
@@ -23001,7 +23206,7 @@
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E27">
         <f t="shared" si="7"/>
@@ -23104,7 +23309,7 @@
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E30">
         <f t="shared" si="7"/>
@@ -23207,7 +23412,7 @@
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E33">
         <f t="shared" si="7"/>
@@ -23310,7 +23515,7 @@
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E36">
         <f t="shared" si="7"/>
@@ -23413,7 +23618,7 @@
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E39">
         <f t="shared" si="7"/>
@@ -23516,7 +23721,7 @@
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E42">
         <f t="shared" si="7"/>
@@ -23619,7 +23824,7 @@
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E45">
         <f t="shared" si="7"/>
@@ -23722,7 +23927,7 @@
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E48">
         <f t="shared" si="7"/>
@@ -23825,7 +24030,7 @@
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D51" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E51">
         <f t="shared" si="7"/>
@@ -23928,7 +24133,7 @@
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D54" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E54">
         <f t="shared" si="7"/>
@@ -24031,7 +24236,7 @@
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D57" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E57">
         <f t="shared" si="7"/>
@@ -24134,7 +24339,7 @@
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D60" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E60">
         <f t="shared" si="7"/>
@@ -24237,7 +24442,7 @@
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D63" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E63">
         <f t="shared" si="7"/>
@@ -24340,7 +24545,7 @@
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D66" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E66">
         <f t="shared" si="7"/>

</xml_diff>

<commit_message>
tighter growth constraint on DAC done properly this time
</commit_message>
<xml_diff>
--- a/suppxls/Scen_UC_ELC.xlsx
+++ b/suppxls/Scen_UC_ELC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\suppxls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF2F4FB2-0B1C-483F-A1B8-2A95D1EC865F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8579AA84-94EF-4D76-9F9A-E76D4B2DC9B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" firstSheet="3" activeTab="6" xr2:uid="{22D7DAD2-FC1B-44BE-801D-D5E60FB61EEE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="6" xr2:uid="{22D7DAD2-FC1B-44BE-801D-D5E60FB61EEE}"/>
   </bookViews>
   <sheets>
     <sheet name="BuildRateConstraints" sheetId="1" r:id="rId1"/>
@@ -21607,10 +21607,10 @@
         <v>1.2</v>
       </c>
       <c r="H21">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="I21">
-        <v>-1000</v>
+        <v>-200</v>
       </c>
       <c r="J21" s="2">
         <v>5</v>
@@ -21638,11 +21638,10 @@
         <v>1.2</v>
       </c>
       <c r="H22">
-        <f>H21</f>
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="I22">
-        <v>-1000</v>
+        <v>-200</v>
       </c>
       <c r="J22" s="2">
         <v>5</v>
@@ -21671,11 +21670,10 @@
         <v>100</v>
       </c>
       <c r="H23">
-        <f>H22</f>
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="I23">
-        <v>-1000</v>
+        <v>-200</v>
       </c>
       <c r="J23" s="2">
         <v>5</v>

</xml_diff>

<commit_message>
Fixes to cost of LCVs, RM and L1 profiles
Need to fix Sets for ELC_OtherInputs (material input), still need to fix profiles for L0 and to add the 3 new growth scenarios
</commit_message>
<xml_diff>
--- a/suppxls/Scen_UC_ELC.xlsx
+++ b/suppxls/Scen_UC_ELC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\suppxls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8579AA84-94EF-4D76-9F9A-E76D4B2DC9B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E37E34-9494-4EB2-BE1E-E513C22704F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="6" xr2:uid="{22D7DAD2-FC1B-44BE-801D-D5E60FB61EEE}"/>
+    <workbookView xWindow="1560" yWindow="-17985" windowWidth="30690" windowHeight="15435" firstSheet="4" activeTab="8" xr2:uid="{22D7DAD2-FC1B-44BE-801D-D5E60FB61EEE}"/>
   </bookViews>
   <sheets>
     <sheet name="BuildRateConstraints" sheetId="1" r:id="rId1"/>
@@ -2021,7 +2021,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="86">
   <si>
     <t>UP</t>
   </si>
@@ -2276,6 +2276,9 @@
   </si>
   <si>
     <t>UDACCO2*</t>
+  </si>
+  <si>
+    <t>TPPRCAROGSH-N</t>
   </si>
 </sst>
 </file>
@@ -19787,9 +19790,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -19827,7 +19830,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -19933,7 +19936,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -20075,7 +20078,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -21016,7 +21019,7 @@
   </sheetPr>
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
@@ -22396,10 +22399,10 @@
   <sheetPr>
     <tabColor theme="8"/>
   </sheetPr>
-  <dimension ref="A1:N68"/>
+  <dimension ref="A1:N71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -22520,7 +22523,7 @@
     </row>
     <row r="7" spans="1:11">
       <c r="B7" s="2" t="str">
-        <f t="shared" ref="B7:B23" si="0">"UC_Growth_"&amp;D7</f>
+        <f t="shared" ref="B7:B26" si="0">"UC_Growth_"&amp;D7</f>
         <v>UC_Growth_TPPRCARELC-N</v>
       </c>
       <c r="C7" s="2" t="str">
@@ -22588,16 +22591,15 @@
     <row r="9" spans="1:11">
       <c r="B9" s="2" t="str">
         <f>"UC_Growth_"&amp;D9</f>
-        <v>UC_Growth_TPPRCARHGNF-N</v>
+        <v>UC_Growth_TPPRCAROGSH-N</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>65</v>
+      <c r="D9" t="s">
+        <v>85</v>
       </c>
       <c r="E9">
-        <f>E6</f>
         <v>2024</v>
       </c>
       <c r="F9" s="2" t="s">
@@ -22621,15 +22623,14 @@
     <row r="10" spans="1:11">
       <c r="B10" s="2" t="str">
         <f t="shared" ref="B10:B11" si="1">"UC_Growth_"&amp;D10</f>
-        <v>UC_Growth_TPPRCARHGNF-N</v>
+        <v>UC_Growth_TPPRCAROGSH-N</v>
       </c>
       <c r="C10" s="2" t="str">
         <f>C9</f>
         <v>NCAP,GROWTH</v>
       </c>
-      <c r="D10" s="2" t="str">
-        <f>D9</f>
-        <v>TPPRCARHGNF-N</v>
+      <c r="D10" t="s">
+        <v>85</v>
       </c>
       <c r="E10">
         <v>2054</v>
@@ -22655,15 +22656,14 @@
     <row r="11" spans="1:11">
       <c r="B11" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>UC_Growth_TPPRCARHGNF-N</v>
+        <v>UC_Growth_TPPRCAROGSH-N</v>
       </c>
       <c r="C11" s="2" t="str">
         <f>C10</f>
         <v>NCAP,GROWTH</v>
       </c>
-      <c r="D11" s="2" t="str">
-        <f>D10</f>
-        <v>TPPRCARHGNF-N</v>
+      <c r="D11" t="s">
+        <v>85</v>
       </c>
       <c r="E11">
         <v>2055</v>
@@ -22688,16 +22688,16 @@
     <row r="12" spans="1:11">
       <c r="B12" s="2" t="str">
         <f>"UC_Growth_"&amp;D12</f>
-        <v>UC_Growth_TPPRSUVELC-N</v>
+        <v>UC_Growth_TPPRCARHGNF-N</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E12">
-        <f>E9</f>
+        <f>E6</f>
         <v>2024</v>
       </c>
       <c r="F12" s="2" t="s">
@@ -22721,7 +22721,7 @@
     <row r="13" spans="1:11">
       <c r="B13" s="2" t="str">
         <f t="shared" ref="B13:B14" si="2">"UC_Growth_"&amp;D13</f>
-        <v>UC_Growth_TPPRSUVELC-N</v>
+        <v>UC_Growth_TPPRCARHGNF-N</v>
       </c>
       <c r="C13" s="2" t="str">
         <f>C12</f>
@@ -22729,7 +22729,7 @@
       </c>
       <c r="D13" s="2" t="str">
         <f>D12</f>
-        <v>TPPRSUVELC-N</v>
+        <v>TPPRCARHGNF-N</v>
       </c>
       <c r="E13">
         <v>2054</v>
@@ -22755,7 +22755,7 @@
     <row r="14" spans="1:11">
       <c r="B14" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>UC_Growth_TPPRSUVELC-N</v>
+        <v>UC_Growth_TPPRCARHGNF-N</v>
       </c>
       <c r="C14" s="2" t="str">
         <f>C13</f>
@@ -22763,7 +22763,7 @@
       </c>
       <c r="D14" s="2" t="str">
         <f>D13</f>
-        <v>TPPRSUVELC-N</v>
+        <v>TPPRCARHGNF-N</v>
       </c>
       <c r="E14">
         <v>2055</v>
@@ -22788,13 +22788,13 @@
     <row r="15" spans="1:11">
       <c r="B15" s="2" t="str">
         <f>"UC_Growth_"&amp;D15</f>
-        <v>UC_Growth_TPPRSUVHGNF-N</v>
+        <v>UC_Growth_TPPRSUVELC-N</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E15">
         <f>E12</f>
@@ -22821,7 +22821,7 @@
     <row r="16" spans="1:11">
       <c r="B16" s="2" t="str">
         <f t="shared" ref="B16:B17" si="3">"UC_Growth_"&amp;D16</f>
-        <v>UC_Growth_TPPRSUVHGNF-N</v>
+        <v>UC_Growth_TPPRSUVELC-N</v>
       </c>
       <c r="C16" s="2" t="str">
         <f>C15</f>
@@ -22829,7 +22829,7 @@
       </c>
       <c r="D16" s="2" t="str">
         <f>D15</f>
-        <v>TPPRSUVHGNF-N</v>
+        <v>TPPRSUVELC-N</v>
       </c>
       <c r="E16">
         <v>2054</v>
@@ -22855,7 +22855,7 @@
     <row r="17" spans="2:14">
       <c r="B17" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>UC_Growth_TPPRSUVHGNF-N</v>
+        <v>UC_Growth_TPPRSUVELC-N</v>
       </c>
       <c r="C17" s="2" t="str">
         <f>C16</f>
@@ -22863,7 +22863,7 @@
       </c>
       <c r="D17" s="2" t="str">
         <f>D16</f>
-        <v>TPPRSUVHGNF-N</v>
+        <v>TPPRSUVELC-N</v>
       </c>
       <c r="E17">
         <v>2055</v>
@@ -22888,16 +22888,16 @@
     <row r="18" spans="2:14">
       <c r="B18" s="2" t="str">
         <f>"UC_Growth_"&amp;D18</f>
-        <v>UC_Growth_TPPUMBTELC-N</v>
+        <v>UC_Growth_TPPRSUVHGNF-N</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E18">
-        <f>$G$1</f>
+        <f>E15</f>
         <v>2024</v>
       </c>
       <c r="F18" s="2" t="s">
@@ -22911,7 +22911,8 @@
         <v>1</v>
       </c>
       <c r="I18">
-        <v>-2</v>
+        <f>-$E$2</f>
+        <v>-10</v>
       </c>
       <c r="J18" s="2">
         <v>5</v>
@@ -22920,7 +22921,7 @@
     <row r="19" spans="2:14">
       <c r="B19" s="2" t="str">
         <f t="shared" ref="B19:B20" si="4">"UC_Growth_"&amp;D19</f>
-        <v>UC_Growth_TPPUMBTELC-N</v>
+        <v>UC_Growth_TPPRSUVHGNF-N</v>
       </c>
       <c r="C19" s="2" t="str">
         <f>C18</f>
@@ -22928,7 +22929,7 @@
       </c>
       <c r="D19" s="2" t="str">
         <f>D18</f>
-        <v>TPPUMBTELC-N</v>
+        <v>TPPRSUVHGNF-N</v>
       </c>
       <c r="E19">
         <v>2054</v>
@@ -22945,7 +22946,7 @@
       </c>
       <c r="I19">
         <f>I18</f>
-        <v>-2</v>
+        <v>-10</v>
       </c>
       <c r="J19" s="2">
         <v>5</v>
@@ -22954,7 +22955,7 @@
     <row r="20" spans="2:14">
       <c r="B20" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>UC_Growth_TPPUMBTELC-N</v>
+        <v>UC_Growth_TPPRSUVHGNF-N</v>
       </c>
       <c r="C20" s="2" t="str">
         <f>C19</f>
@@ -22962,7 +22963,7 @@
       </c>
       <c r="D20" s="2" t="str">
         <f>D19</f>
-        <v>TPPUMBTELC-N</v>
+        <v>TPPRSUVHGNF-N</v>
       </c>
       <c r="E20">
         <v>2055</v>
@@ -22978,7 +22979,7 @@
       </c>
       <c r="I20">
         <f>I19</f>
-        <v>-2</v>
+        <v>-10</v>
       </c>
       <c r="J20" s="2">
         <v>5</v>
@@ -22986,18 +22987,17 @@
     </row>
     <row r="21" spans="2:14">
       <c r="B21" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UC_Growth_TFLCVOGSH-N</v>
-      </c>
-      <c r="C21" s="2" t="str">
-        <f>C8</f>
-        <v>NCAP,GROWTH</v>
+        <f>"UC_Growth_"&amp;D21</f>
+        <v>UC_Growth_TPPUMBTELC-N</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E21">
-        <f>E6</f>
+        <f>$G$1</f>
         <v>2024</v>
       </c>
       <c r="F21" s="2" t="s">
@@ -23011,29 +23011,26 @@
         <v>1</v>
       </c>
       <c r="I21">
-        <f>-$E$2</f>
-        <v>-10</v>
+        <v>-2</v>
       </c>
       <c r="J21" s="2">
         <v>5</v>
       </c>
-      <c r="N21" s="2"/>
     </row>
     <row r="22" spans="2:14">
       <c r="B22" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UC_Growth_TFLCVOGSH-N</v>
+        <f t="shared" ref="B22:B23" si="5">"UC_Growth_"&amp;D22</f>
+        <v>UC_Growth_TPPUMBTELC-N</v>
       </c>
       <c r="C22" s="2" t="str">
-        <f t="shared" ref="C22:C26" si="5">C21</f>
+        <f>C21</f>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D22" s="2" t="str">
         <f>D21</f>
-        <v>TFLCVOGSH-N</v>
+        <v>TPPUMBTELC-N</v>
       </c>
       <c r="E22">
-        <f>E7</f>
         <v>2054</v>
       </c>
       <c r="F22" s="2" t="s">
@@ -23048,28 +23045,26 @@
       </c>
       <c r="I22">
         <f>I21</f>
-        <v>-10</v>
+        <v>-2</v>
       </c>
       <c r="J22" s="2">
         <v>5</v>
       </c>
-      <c r="N22" s="2"/>
     </row>
     <row r="23" spans="2:14">
       <c r="B23" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UC_Growth_TFLCVOGSH-N</v>
+        <f t="shared" si="5"/>
+        <v>UC_Growth_TPPUMBTELC-N</v>
       </c>
       <c r="C23" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f>C22</f>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D23" s="2" t="str">
         <f>D22</f>
-        <v>TFLCVOGSH-N</v>
+        <v>TPPUMBTELC-N</v>
       </c>
       <c r="E23">
-        <f>E8</f>
         <v>2055</v>
       </c>
       <c r="F23" s="2" t="s">
@@ -23083,27 +23078,26 @@
       </c>
       <c r="I23">
         <f>I22</f>
-        <v>-10</v>
+        <v>-2</v>
       </c>
       <c r="J23" s="2">
         <v>5</v>
       </c>
-      <c r="N23" s="2"/>
     </row>
     <row r="24" spans="2:14">
       <c r="B24" s="2" t="str">
-        <f t="shared" ref="B24:B26" si="6">"UC_Growth_"&amp;D24</f>
-        <v>UC_Growth_TFLCVELC-N</v>
+        <f t="shared" si="0"/>
+        <v>UC_Growth_TFLCVOGSH-N</v>
       </c>
       <c r="C24" s="2" t="str">
-        <f>C20</f>
+        <f>C8</f>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E24">
-        <f t="shared" ref="E24:E68" si="7">E18</f>
+        <f>E6</f>
         <v>2024</v>
       </c>
       <c r="F24" s="2" t="s">
@@ -23127,19 +23121,19 @@
     </row>
     <row r="25" spans="2:14">
       <c r="B25" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v>UC_Growth_TFLCVELC-N</v>
+        <f t="shared" si="0"/>
+        <v>UC_Growth_TFLCVOGSH-N</v>
       </c>
       <c r="C25" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="C25:C29" si="6">C24</f>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D25" s="2" t="str">
         <f>D24</f>
-        <v>TFLCVELC-N</v>
+        <v>TFLCVOGSH-N</v>
       </c>
       <c r="E25">
-        <f t="shared" si="7"/>
+        <f>E7</f>
         <v>2054</v>
       </c>
       <c r="F25" s="2" t="s">
@@ -23163,19 +23157,19 @@
     </row>
     <row r="26" spans="2:14">
       <c r="B26" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>UC_Growth_TFLCVOGSH-N</v>
+      </c>
+      <c r="C26" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>UC_Growth_TFLCVELC-N</v>
-      </c>
-      <c r="C26" s="2" t="str">
-        <f t="shared" si="5"/>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D26" s="2" t="str">
         <f>D25</f>
-        <v>TFLCVELC-N</v>
+        <v>TFLCVOGSH-N</v>
       </c>
       <c r="E26">
-        <f t="shared" si="7"/>
+        <f>E8</f>
         <v>2055</v>
       </c>
       <c r="F26" s="2" t="s">
@@ -23198,18 +23192,18 @@
     </row>
     <row r="27" spans="2:14">
       <c r="B27" s="2" t="str">
-        <f t="shared" ref="B27:B29" si="8">"UC_Growth_"&amp;D27</f>
-        <v>UC_Growth_TFHCV1ELC-N</v>
+        <f t="shared" ref="B27:B29" si="7">"UC_Growth_"&amp;D27</f>
+        <v>UC_Growth_TFLCVELC-N</v>
       </c>
       <c r="C27" s="2" t="str">
         <f>C23</f>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E27">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="E27:E71" si="8">E21</f>
         <v>2024</v>
       </c>
       <c r="F27" s="2" t="s">
@@ -23223,7 +23217,8 @@
         <v>1</v>
       </c>
       <c r="I27">
-        <v>-5</v>
+        <f>-$E$2</f>
+        <v>-10</v>
       </c>
       <c r="J27" s="2">
         <v>5</v>
@@ -23232,19 +23227,19 @@
     </row>
     <row r="28" spans="2:14">
       <c r="B28" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v>UC_Growth_TFHCV1ELC-N</v>
+        <f t="shared" si="7"/>
+        <v>UC_Growth_TFLCVELC-N</v>
       </c>
       <c r="C28" s="2" t="str">
-        <f t="shared" ref="C28:C68" si="9">C27</f>
+        <f t="shared" si="6"/>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D28" s="2" t="str">
         <f>D27</f>
-        <v>TFHCV1ELC-N</v>
+        <v>TFLCVELC-N</v>
       </c>
       <c r="E28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2054</v>
       </c>
       <c r="F28" s="2" t="s">
@@ -23259,27 +23254,28 @@
       </c>
       <c r="I28">
         <f>I27</f>
-        <v>-5</v>
+        <v>-10</v>
       </c>
       <c r="J28" s="2">
         <v>5</v>
       </c>
+      <c r="N28" s="2"/>
     </row>
     <row r="29" spans="2:14">
       <c r="B29" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v>UC_Growth_TFHCV1ELC-N</v>
+        <f t="shared" si="7"/>
+        <v>UC_Growth_TFLCVELC-N</v>
       </c>
       <c r="C29" s="2" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D29" s="2" t="str">
         <f>D28</f>
-        <v>TFHCV1ELC-N</v>
+        <v>TFLCVELC-N</v>
       </c>
       <c r="E29">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2055</v>
       </c>
       <c r="F29" s="2" t="s">
@@ -23293,26 +23289,27 @@
       </c>
       <c r="I29">
         <f>I28</f>
-        <v>-5</v>
+        <v>-10</v>
       </c>
       <c r="J29" s="2">
         <v>5</v>
       </c>
+      <c r="N29" s="2"/>
     </row>
     <row r="30" spans="2:14">
       <c r="B30" s="2" t="str">
-        <f t="shared" ref="B30:B50" si="10">"UC_Growth_"&amp;D30</f>
-        <v>UC_Growth_TFHCV2ELC-N</v>
+        <f t="shared" ref="B30:B32" si="9">"UC_Growth_"&amp;D30</f>
+        <v>UC_Growth_TFHCV1ELC-N</v>
       </c>
       <c r="C30" s="2" t="str">
         <f>C26</f>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2024</v>
       </c>
       <c r="F30" s="2" t="s">
@@ -23326,7 +23323,7 @@
         <v>1</v>
       </c>
       <c r="I30">
-        <v>-2</v>
+        <v>-5</v>
       </c>
       <c r="J30" s="2">
         <v>5</v>
@@ -23335,19 +23332,19 @@
     </row>
     <row r="31" spans="2:14">
       <c r="B31" s="2" t="str">
-        <f t="shared" si="10"/>
-        <v>UC_Growth_TFHCV2ELC-N</v>
+        <f t="shared" si="9"/>
+        <v>UC_Growth_TFHCV1ELC-N</v>
       </c>
       <c r="C31" s="2" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="C31:C71" si="10">C30</f>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D31" s="2" t="str">
         <f>D30</f>
-        <v>TFHCV2ELC-N</v>
+        <v>TFHCV1ELC-N</v>
       </c>
       <c r="E31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2054</v>
       </c>
       <c r="F31" s="2" t="s">
@@ -23362,7 +23359,7 @@
       </c>
       <c r="I31">
         <f>I30</f>
-        <v>-2</v>
+        <v>-5</v>
       </c>
       <c r="J31" s="2">
         <v>5</v>
@@ -23370,19 +23367,19 @@
     </row>
     <row r="32" spans="2:14">
       <c r="B32" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>UC_Growth_TFHCV1ELC-N</v>
+      </c>
+      <c r="C32" s="2" t="str">
         <f t="shared" si="10"/>
-        <v>UC_Growth_TFHCV2ELC-N</v>
-      </c>
-      <c r="C32" s="2" t="str">
-        <f t="shared" si="9"/>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D32" s="2" t="str">
         <f>D31</f>
-        <v>TFHCV2ELC-N</v>
+        <v>TFHCV1ELC-N</v>
       </c>
       <c r="E32">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2055</v>
       </c>
       <c r="F32" s="2" t="s">
@@ -23396,7 +23393,7 @@
       </c>
       <c r="I32">
         <f>I31</f>
-        <v>-2</v>
+        <v>-5</v>
       </c>
       <c r="J32" s="2">
         <v>5</v>
@@ -23404,18 +23401,18 @@
     </row>
     <row r="33" spans="2:14">
       <c r="B33" s="2" t="str">
-        <f t="shared" si="10"/>
-        <v>UC_Growth_TFHCV3ELC-N</v>
+        <f t="shared" ref="B33:B53" si="11">"UC_Growth_"&amp;D33</f>
+        <v>UC_Growth_TFHCV2ELC-N</v>
       </c>
       <c r="C33" s="2" t="str">
         <f>C29</f>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2024</v>
       </c>
       <c r="F33" s="2" t="s">
@@ -23438,19 +23435,19 @@
     </row>
     <row r="34" spans="2:14">
       <c r="B34" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>UC_Growth_TFHCV2ELC-N</v>
+      </c>
+      <c r="C34" s="2" t="str">
         <f t="shared" si="10"/>
-        <v>UC_Growth_TFHCV3ELC-N</v>
-      </c>
-      <c r="C34" s="2" t="str">
-        <f t="shared" si="9"/>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D34" s="2" t="str">
         <f>D33</f>
-        <v>TFHCV3ELC-N</v>
+        <v>TFHCV2ELC-N</v>
       </c>
       <c r="E34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2054</v>
       </c>
       <c r="F34" s="2" t="s">
@@ -23473,19 +23470,19 @@
     </row>
     <row r="35" spans="2:14">
       <c r="B35" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>UC_Growth_TFHCV2ELC-N</v>
+      </c>
+      <c r="C35" s="2" t="str">
         <f t="shared" si="10"/>
-        <v>UC_Growth_TFHCV3ELC-N</v>
-      </c>
-      <c r="C35" s="2" t="str">
-        <f t="shared" si="9"/>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D35" s="2" t="str">
         <f>D34</f>
-        <v>TFHCV3ELC-N</v>
+        <v>TFHCV2ELC-N</v>
       </c>
       <c r="E35">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2055</v>
       </c>
       <c r="F35" s="2" t="s">
@@ -23507,18 +23504,18 @@
     </row>
     <row r="36" spans="2:14">
       <c r="B36" s="2" t="str">
-        <f t="shared" si="10"/>
-        <v>UC_Growth_TFHCV4ELC-N</v>
+        <f t="shared" si="11"/>
+        <v>UC_Growth_TFHCV3ELC-N</v>
       </c>
       <c r="C36" s="2" t="str">
         <f>C32</f>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E36">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2024</v>
       </c>
       <c r="F36" s="2" t="s">
@@ -23541,19 +23538,19 @@
     </row>
     <row r="37" spans="2:14">
       <c r="B37" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>UC_Growth_TFHCV3ELC-N</v>
+      </c>
+      <c r="C37" s="2" t="str">
         <f t="shared" si="10"/>
-        <v>UC_Growth_TFHCV4ELC-N</v>
-      </c>
-      <c r="C37" s="2" t="str">
-        <f t="shared" si="9"/>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D37" s="2" t="str">
         <f>D36</f>
-        <v>TFHCV4ELC-N</v>
+        <v>TFHCV3ELC-N</v>
       </c>
       <c r="E37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2054</v>
       </c>
       <c r="F37" s="2" t="s">
@@ -23576,19 +23573,19 @@
     </row>
     <row r="38" spans="2:14">
       <c r="B38" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>UC_Growth_TFHCV3ELC-N</v>
+      </c>
+      <c r="C38" s="2" t="str">
         <f t="shared" si="10"/>
-        <v>UC_Growth_TFHCV4ELC-N</v>
-      </c>
-      <c r="C38" s="2" t="str">
-        <f t="shared" si="9"/>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D38" s="2" t="str">
         <f>D37</f>
-        <v>TFHCV4ELC-N</v>
+        <v>TFHCV3ELC-N</v>
       </c>
       <c r="E38">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2055</v>
       </c>
       <c r="F38" s="2" t="s">
@@ -23610,18 +23607,18 @@
     </row>
     <row r="39" spans="2:14">
       <c r="B39" s="2" t="str">
-        <f t="shared" si="10"/>
-        <v>UC_Growth_TFHCV5ELC-N</v>
+        <f t="shared" si="11"/>
+        <v>UC_Growth_TFHCV4ELC-N</v>
       </c>
       <c r="C39" s="2" t="str">
         <f>C35</f>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E39">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2024</v>
       </c>
       <c r="F39" s="2" t="s">
@@ -23644,19 +23641,19 @@
     </row>
     <row r="40" spans="2:14">
       <c r="B40" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>UC_Growth_TFHCV4ELC-N</v>
+      </c>
+      <c r="C40" s="2" t="str">
         <f t="shared" si="10"/>
-        <v>UC_Growth_TFHCV5ELC-N</v>
-      </c>
-      <c r="C40" s="2" t="str">
-        <f t="shared" si="9"/>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D40" s="2" t="str">
         <f>D39</f>
-        <v>TFHCV5ELC-N</v>
+        <v>TFHCV4ELC-N</v>
       </c>
       <c r="E40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2054</v>
       </c>
       <c r="F40" s="2" t="s">
@@ -23679,19 +23676,19 @@
     </row>
     <row r="41" spans="2:14">
       <c r="B41" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>UC_Growth_TFHCV4ELC-N</v>
+      </c>
+      <c r="C41" s="2" t="str">
         <f t="shared" si="10"/>
-        <v>UC_Growth_TFHCV5ELC-N</v>
-      </c>
-      <c r="C41" s="2" t="str">
-        <f t="shared" si="9"/>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D41" s="2" t="str">
         <f>D40</f>
-        <v>TFHCV5ELC-N</v>
+        <v>TFHCV4ELC-N</v>
       </c>
       <c r="E41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2055</v>
       </c>
       <c r="F41" s="2" t="s">
@@ -23713,18 +23710,18 @@
     </row>
     <row r="42" spans="2:14">
       <c r="B42" s="2" t="str">
-        <f t="shared" si="10"/>
-        <v>UC_Growth_TFHCV6ELC-N</v>
+        <f t="shared" si="11"/>
+        <v>UC_Growth_TFHCV5ELC-N</v>
       </c>
       <c r="C42" s="2" t="str">
         <f>C38</f>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E42">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2024</v>
       </c>
       <c r="F42" s="2" t="s">
@@ -23747,19 +23744,19 @@
     </row>
     <row r="43" spans="2:14">
       <c r="B43" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>UC_Growth_TFHCV5ELC-N</v>
+      </c>
+      <c r="C43" s="2" t="str">
         <f t="shared" si="10"/>
-        <v>UC_Growth_TFHCV6ELC-N</v>
-      </c>
-      <c r="C43" s="2" t="str">
-        <f t="shared" si="9"/>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D43" s="2" t="str">
         <f>D42</f>
-        <v>TFHCV6ELC-N</v>
+        <v>TFHCV5ELC-N</v>
       </c>
       <c r="E43">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2054</v>
       </c>
       <c r="F43" s="2" t="s">
@@ -23782,19 +23779,19 @@
     </row>
     <row r="44" spans="2:14">
       <c r="B44" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>UC_Growth_TFHCV5ELC-N</v>
+      </c>
+      <c r="C44" s="2" t="str">
         <f t="shared" si="10"/>
-        <v>UC_Growth_TFHCV6ELC-N</v>
-      </c>
-      <c r="C44" s="2" t="str">
-        <f t="shared" si="9"/>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D44" s="2" t="str">
         <f>D43</f>
-        <v>TFHCV6ELC-N</v>
+        <v>TFHCV5ELC-N</v>
       </c>
       <c r="E44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2055</v>
       </c>
       <c r="F44" s="2" t="s">
@@ -23816,18 +23813,18 @@
     </row>
     <row r="45" spans="2:14">
       <c r="B45" s="2" t="str">
-        <f t="shared" si="10"/>
-        <v>UC_Growth_TFHCV7ELC-N</v>
+        <f t="shared" si="11"/>
+        <v>UC_Growth_TFHCV6ELC-N</v>
       </c>
       <c r="C45" s="2" t="str">
         <f>C41</f>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E45">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2024</v>
       </c>
       <c r="F45" s="2" t="s">
@@ -23850,19 +23847,19 @@
     </row>
     <row r="46" spans="2:14">
       <c r="B46" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>UC_Growth_TFHCV6ELC-N</v>
+      </c>
+      <c r="C46" s="2" t="str">
         <f t="shared" si="10"/>
-        <v>UC_Growth_TFHCV7ELC-N</v>
-      </c>
-      <c r="C46" s="2" t="str">
-        <f t="shared" si="9"/>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D46" s="2" t="str">
         <f>D45</f>
-        <v>TFHCV7ELC-N</v>
+        <v>TFHCV6ELC-N</v>
       </c>
       <c r="E46">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2054</v>
       </c>
       <c r="F46" s="2" t="s">
@@ -23885,19 +23882,19 @@
     </row>
     <row r="47" spans="2:14">
       <c r="B47" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>UC_Growth_TFHCV6ELC-N</v>
+      </c>
+      <c r="C47" s="2" t="str">
         <f t="shared" si="10"/>
-        <v>UC_Growth_TFHCV7ELC-N</v>
-      </c>
-      <c r="C47" s="2" t="str">
-        <f t="shared" si="9"/>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D47" s="2" t="str">
         <f>D46</f>
-        <v>TFHCV7ELC-N</v>
+        <v>TFHCV6ELC-N</v>
       </c>
       <c r="E47">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2055</v>
       </c>
       <c r="F47" s="2" t="s">
@@ -23919,18 +23916,18 @@
     </row>
     <row r="48" spans="2:14">
       <c r="B48" s="2" t="str">
-        <f t="shared" si="10"/>
-        <v>UC_Growth_TFHCV1ELC-N</v>
+        <f t="shared" si="11"/>
+        <v>UC_Growth_TFHCV7ELC-N</v>
       </c>
       <c r="C48" s="2" t="str">
         <f>C44</f>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="E48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2024</v>
       </c>
       <c r="F48" s="2" t="s">
@@ -23944,7 +23941,7 @@
         <v>1</v>
       </c>
       <c r="I48">
-        <v>-5</v>
+        <v>-2</v>
       </c>
       <c r="J48" s="2">
         <v>5</v>
@@ -23953,19 +23950,19 @@
     </row>
     <row r="49" spans="2:14">
       <c r="B49" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>UC_Growth_TFHCV7ELC-N</v>
+      </c>
+      <c r="C49" s="2" t="str">
         <f t="shared" si="10"/>
-        <v>UC_Growth_TFHCV1ELC-N</v>
-      </c>
-      <c r="C49" s="2" t="str">
-        <f t="shared" si="9"/>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D49" s="2" t="str">
         <f>D48</f>
-        <v>TFHCV1ELC-N</v>
+        <v>TFHCV7ELC-N</v>
       </c>
       <c r="E49">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2054</v>
       </c>
       <c r="F49" s="2" t="s">
@@ -23980,7 +23977,7 @@
       </c>
       <c r="I49">
         <f>I48</f>
-        <v>-5</v>
+        <v>-2</v>
       </c>
       <c r="J49" s="2">
         <v>5</v>
@@ -23988,19 +23985,19 @@
     </row>
     <row r="50" spans="2:14">
       <c r="B50" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>UC_Growth_TFHCV7ELC-N</v>
+      </c>
+      <c r="C50" s="2" t="str">
         <f t="shared" si="10"/>
-        <v>UC_Growth_TFHCV1ELC-N</v>
-      </c>
-      <c r="C50" s="2" t="str">
-        <f t="shared" si="9"/>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D50" s="2" t="str">
         <f>D49</f>
-        <v>TFHCV1ELC-N</v>
+        <v>TFHCV7ELC-N</v>
       </c>
       <c r="E50">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2055</v>
       </c>
       <c r="F50" s="2" t="s">
@@ -24014,7 +24011,7 @@
       </c>
       <c r="I50">
         <f>I49</f>
-        <v>-5</v>
+        <v>-2</v>
       </c>
       <c r="J50" s="2">
         <v>5</v>
@@ -24022,18 +24019,18 @@
     </row>
     <row r="51" spans="2:14">
       <c r="B51" s="2" t="str">
-        <f t="shared" ref="B51:B68" si="11">"UC_Growth_"&amp;D51</f>
-        <v>UC_Growth_TFHCV2HGN-N</v>
+        <f t="shared" si="11"/>
+        <v>UC_Growth_TFHCV1ELC-N</v>
       </c>
       <c r="C51" s="2" t="str">
         <f>C47</f>
         <v>NCAP,GROWTH</v>
       </c>
-      <c r="D51" t="s">
-        <v>74</v>
+      <c r="D51" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="E51">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2024</v>
       </c>
       <c r="F51" s="2" t="s">
@@ -24047,7 +24044,7 @@
         <v>1</v>
       </c>
       <c r="I51">
-        <v>-2</v>
+        <v>-5</v>
       </c>
       <c r="J51" s="2">
         <v>5</v>
@@ -24057,18 +24054,18 @@
     <row r="52" spans="2:14">
       <c r="B52" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>UC_Growth_TFHCV2HGN-N</v>
+        <v>UC_Growth_TFHCV1ELC-N</v>
       </c>
       <c r="C52" s="2" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D52" s="2" t="str">
         <f>D51</f>
-        <v>TFHCV2HGN-N</v>
+        <v>TFHCV1ELC-N</v>
       </c>
       <c r="E52">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2054</v>
       </c>
       <c r="F52" s="2" t="s">
@@ -24083,7 +24080,7 @@
       </c>
       <c r="I52">
         <f>I51</f>
-        <v>-2</v>
+        <v>-5</v>
       </c>
       <c r="J52" s="2">
         <v>5</v>
@@ -24092,18 +24089,18 @@
     <row r="53" spans="2:14">
       <c r="B53" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>UC_Growth_TFHCV2HGN-N</v>
+        <v>UC_Growth_TFHCV1ELC-N</v>
       </c>
       <c r="C53" s="2" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D53" s="2" t="str">
         <f>D52</f>
-        <v>TFHCV2HGN-N</v>
+        <v>TFHCV1ELC-N</v>
       </c>
       <c r="E53">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2055</v>
       </c>
       <c r="F53" s="2" t="s">
@@ -24117,7 +24114,7 @@
       </c>
       <c r="I53">
         <f>I52</f>
-        <v>-2</v>
+        <v>-5</v>
       </c>
       <c r="J53" s="2">
         <v>5</v>
@@ -24125,18 +24122,18 @@
     </row>
     <row r="54" spans="2:14">
       <c r="B54" s="2" t="str">
-        <f t="shared" si="11"/>
-        <v>UC_Growth_TFHCV3HGN-N</v>
+        <f t="shared" ref="B54:B71" si="12">"UC_Growth_"&amp;D54</f>
+        <v>UC_Growth_TFHCV2HGN-N</v>
       </c>
       <c r="C54" s="2" t="str">
         <f>C50</f>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D54" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E54">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2024</v>
       </c>
       <c r="F54" s="2" t="s">
@@ -24159,19 +24156,19 @@
     </row>
     <row r="55" spans="2:14">
       <c r="B55" s="2" t="str">
-        <f t="shared" si="11"/>
-        <v>UC_Growth_TFHCV3HGN-N</v>
+        <f t="shared" si="12"/>
+        <v>UC_Growth_TFHCV2HGN-N</v>
       </c>
       <c r="C55" s="2" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D55" s="2" t="str">
         <f>D54</f>
-        <v>TFHCV3HGN-N</v>
+        <v>TFHCV2HGN-N</v>
       </c>
       <c r="E55">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2054</v>
       </c>
       <c r="F55" s="2" t="s">
@@ -24194,19 +24191,19 @@
     </row>
     <row r="56" spans="2:14">
       <c r="B56" s="2" t="str">
-        <f t="shared" si="11"/>
-        <v>UC_Growth_TFHCV3HGN-N</v>
+        <f t="shared" si="12"/>
+        <v>UC_Growth_TFHCV2HGN-N</v>
       </c>
       <c r="C56" s="2" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D56" s="2" t="str">
         <f>D55</f>
-        <v>TFHCV3HGN-N</v>
+        <v>TFHCV2HGN-N</v>
       </c>
       <c r="E56">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2055</v>
       </c>
       <c r="F56" s="2" t="s">
@@ -24228,18 +24225,18 @@
     </row>
     <row r="57" spans="2:14">
       <c r="B57" s="2" t="str">
-        <f t="shared" si="11"/>
-        <v>UC_Growth_TFHCV4HGN-N</v>
+        <f t="shared" si="12"/>
+        <v>UC_Growth_TFHCV3HGN-N</v>
       </c>
       <c r="C57" s="2" t="str">
         <f>C53</f>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D57" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E57">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2024</v>
       </c>
       <c r="F57" s="2" t="s">
@@ -24262,19 +24259,19 @@
     </row>
     <row r="58" spans="2:14">
       <c r="B58" s="2" t="str">
-        <f t="shared" si="11"/>
-        <v>UC_Growth_TFHCV4HGN-N</v>
+        <f t="shared" si="12"/>
+        <v>UC_Growth_TFHCV3HGN-N</v>
       </c>
       <c r="C58" s="2" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D58" s="2" t="str">
         <f>D57</f>
-        <v>TFHCV4HGN-N</v>
+        <v>TFHCV3HGN-N</v>
       </c>
       <c r="E58">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2054</v>
       </c>
       <c r="F58" s="2" t="s">
@@ -24297,19 +24294,19 @@
     </row>
     <row r="59" spans="2:14">
       <c r="B59" s="2" t="str">
-        <f t="shared" si="11"/>
-        <v>UC_Growth_TFHCV4HGN-N</v>
+        <f t="shared" si="12"/>
+        <v>UC_Growth_TFHCV3HGN-N</v>
       </c>
       <c r="C59" s="2" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D59" s="2" t="str">
         <f>D58</f>
-        <v>TFHCV4HGN-N</v>
+        <v>TFHCV3HGN-N</v>
       </c>
       <c r="E59">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2055</v>
       </c>
       <c r="F59" s="2" t="s">
@@ -24331,18 +24328,18 @@
     </row>
     <row r="60" spans="2:14">
       <c r="B60" s="2" t="str">
-        <f t="shared" si="11"/>
-        <v>UC_Growth_TFHCV5HGN-N</v>
+        <f t="shared" si="12"/>
+        <v>UC_Growth_TFHCV4HGN-N</v>
       </c>
       <c r="C60" s="2" t="str">
         <f>C56</f>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D60" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E60">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2024</v>
       </c>
       <c r="F60" s="2" t="s">
@@ -24365,19 +24362,19 @@
     </row>
     <row r="61" spans="2:14">
       <c r="B61" s="2" t="str">
-        <f t="shared" si="11"/>
-        <v>UC_Growth_TFHCV5HGN-N</v>
+        <f t="shared" si="12"/>
+        <v>UC_Growth_TFHCV4HGN-N</v>
       </c>
       <c r="C61" s="2" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D61" s="2" t="str">
         <f>D60</f>
-        <v>TFHCV5HGN-N</v>
+        <v>TFHCV4HGN-N</v>
       </c>
       <c r="E61">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2054</v>
       </c>
       <c r="F61" s="2" t="s">
@@ -24400,19 +24397,19 @@
     </row>
     <row r="62" spans="2:14">
       <c r="B62" s="2" t="str">
-        <f t="shared" si="11"/>
-        <v>UC_Growth_TFHCV5HGN-N</v>
+        <f t="shared" si="12"/>
+        <v>UC_Growth_TFHCV4HGN-N</v>
       </c>
       <c r="C62" s="2" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D62" s="2" t="str">
         <f>D61</f>
-        <v>TFHCV5HGN-N</v>
+        <v>TFHCV4HGN-N</v>
       </c>
       <c r="E62">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2055</v>
       </c>
       <c r="F62" s="2" t="s">
@@ -24434,18 +24431,18 @@
     </row>
     <row r="63" spans="2:14">
       <c r="B63" s="2" t="str">
-        <f t="shared" si="11"/>
-        <v>UC_Growth_TFHCV6HGN-N</v>
+        <f t="shared" si="12"/>
+        <v>UC_Growth_TFHCV5HGN-N</v>
       </c>
       <c r="C63" s="2" t="str">
         <f>C59</f>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D63" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E63">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2024</v>
       </c>
       <c r="F63" s="2" t="s">
@@ -24468,19 +24465,19 @@
     </row>
     <row r="64" spans="2:14">
       <c r="B64" s="2" t="str">
-        <f t="shared" si="11"/>
-        <v>UC_Growth_TFHCV6HGN-N</v>
+        <f t="shared" si="12"/>
+        <v>UC_Growth_TFHCV5HGN-N</v>
       </c>
       <c r="C64" s="2" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D64" s="2" t="str">
         <f>D63</f>
-        <v>TFHCV6HGN-N</v>
+        <v>TFHCV5HGN-N</v>
       </c>
       <c r="E64">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2054</v>
       </c>
       <c r="F64" s="2" t="s">
@@ -24503,19 +24500,19 @@
     </row>
     <row r="65" spans="2:14">
       <c r="B65" s="2" t="str">
-        <f t="shared" si="11"/>
-        <v>UC_Growth_TFHCV6HGN-N</v>
+        <f t="shared" si="12"/>
+        <v>UC_Growth_TFHCV5HGN-N</v>
       </c>
       <c r="C65" s="2" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D65" s="2" t="str">
         <f>D64</f>
-        <v>TFHCV6HGN-N</v>
+        <v>TFHCV5HGN-N</v>
       </c>
       <c r="E65">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2055</v>
       </c>
       <c r="F65" s="2" t="s">
@@ -24537,18 +24534,18 @@
     </row>
     <row r="66" spans="2:14">
       <c r="B66" s="2" t="str">
-        <f t="shared" si="11"/>
-        <v>UC_Growth_TFHCV7HGN-N</v>
+        <f t="shared" si="12"/>
+        <v>UC_Growth_TFHCV6HGN-N</v>
       </c>
       <c r="C66" s="2" t="str">
         <f>C62</f>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D66" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E66">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2024</v>
       </c>
       <c r="F66" s="2" t="s">
@@ -24571,19 +24568,19 @@
     </row>
     <row r="67" spans="2:14">
       <c r="B67" s="2" t="str">
-        <f t="shared" si="11"/>
-        <v>UC_Growth_TFHCV7HGN-N</v>
+        <f t="shared" si="12"/>
+        <v>UC_Growth_TFHCV6HGN-N</v>
       </c>
       <c r="C67" s="2" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D67" s="2" t="str">
         <f>D66</f>
-        <v>TFHCV7HGN-N</v>
+        <v>TFHCV6HGN-N</v>
       </c>
       <c r="E67">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2054</v>
       </c>
       <c r="F67" s="2" t="s">
@@ -24606,19 +24603,19 @@
     </row>
     <row r="68" spans="2:14">
       <c r="B68" s="2" t="str">
-        <f t="shared" si="11"/>
-        <v>UC_Growth_TFHCV7HGN-N</v>
+        <f t="shared" si="12"/>
+        <v>UC_Growth_TFHCV6HGN-N</v>
       </c>
       <c r="C68" s="2" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>NCAP,GROWTH</v>
       </c>
       <c r="D68" s="2" t="str">
         <f>D67</f>
-        <v>TFHCV7HGN-N</v>
+        <v>TFHCV6HGN-N</v>
       </c>
       <c r="E68">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2055</v>
       </c>
       <c r="F68" s="2" t="s">
@@ -24635,6 +24632,109 @@
         <v>-2</v>
       </c>
       <c r="J68" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="2:14">
+      <c r="B69" s="2" t="str">
+        <f t="shared" si="12"/>
+        <v>UC_Growth_TFHCV7HGN-N</v>
+      </c>
+      <c r="C69" s="2" t="str">
+        <f>C65</f>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D69" t="s">
+        <v>79</v>
+      </c>
+      <c r="E69">
+        <f t="shared" si="8"/>
+        <v>2024</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G69">
+        <f>1+$E$1</f>
+        <v>1.2</v>
+      </c>
+      <c r="H69">
+        <v>1</v>
+      </c>
+      <c r="I69">
+        <v>-2</v>
+      </c>
+      <c r="J69" s="2">
+        <v>5</v>
+      </c>
+      <c r="N69" s="2"/>
+    </row>
+    <row r="70" spans="2:14">
+      <c r="B70" s="2" t="str">
+        <f t="shared" si="12"/>
+        <v>UC_Growth_TFHCV7HGN-N</v>
+      </c>
+      <c r="C70" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D70" s="2" t="str">
+        <f>D69</f>
+        <v>TFHCV7HGN-N</v>
+      </c>
+      <c r="E70">
+        <f t="shared" si="8"/>
+        <v>2054</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G70">
+        <f>1+$E$1</f>
+        <v>1.2</v>
+      </c>
+      <c r="H70">
+        <v>1</v>
+      </c>
+      <c r="I70">
+        <f>I69</f>
+        <v>-2</v>
+      </c>
+      <c r="J70" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="2:14">
+      <c r="B71" s="2" t="str">
+        <f t="shared" si="12"/>
+        <v>UC_Growth_TFHCV7HGN-N</v>
+      </c>
+      <c r="C71" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>NCAP,GROWTH</v>
+      </c>
+      <c r="D71" s="2" t="str">
+        <f>D70</f>
+        <v>TFHCV7HGN-N</v>
+      </c>
+      <c r="E71">
+        <f t="shared" si="8"/>
+        <v>2055</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G71">
+        <v>100</v>
+      </c>
+      <c r="H71">
+        <v>1</v>
+      </c>
+      <c r="I71">
+        <f>I70</f>
+        <v>-2</v>
+      </c>
+      <c r="J71" s="2">
         <v>5</v>
       </c>
     </row>

</xml_diff>